<commit_message>
Atualização automática da planilha via Apps Script
</commit_message>
<xml_diff>
--- a/Controle_Lote_Validade.xlsx
+++ b/Controle_Lote_Validade.xlsx
@@ -226,7 +226,7 @@
     <t>AGUA PERFUMADA PATCHOULI VANILLA - 1L</t>
   </si>
   <si>
-    <t>J2261</t>
+    <t>testefodase</t>
   </si>
   <si>
     <t>107033500</t>
@@ -3506,7 +3506,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3541,7 +3541,7 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
@@ -3553,6 +3553,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1"/>
@@ -5284,7 +5287,7 @@
       <c r="B105" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C105" s="16" t="s">
         <v>308</v>
       </c>
       <c r="D105" s="8" t="s">
@@ -5536,7 +5539,7 @@
       <c r="B123" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="C123" s="11" t="s">
+      <c r="C123" s="16" t="s">
         <v>360</v>
       </c>
       <c r="D123" s="8" t="s">
@@ -5664,7 +5667,7 @@
       <c r="B133" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C133" s="11" t="s">
+      <c r="C133" s="16" t="s">
         <v>385</v>
       </c>
       <c r="D133" s="8" t="s">
@@ -5818,7 +5821,7 @@
       <c r="B144" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="C144" s="11" t="s">
+      <c r="C144" s="16" t="s">
         <v>417</v>
       </c>
       <c r="D144" s="8" t="s">
@@ -5882,193 +5885,193 @@
       </c>
     </row>
     <row r="149" ht="14.25" customHeight="1">
-      <c r="A149" s="16" t="s">
+      <c r="A149" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="B149" s="16" t="s">
+      <c r="B149" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="C149" s="17" t="str">
+      <c r="C149" s="18" t="str">
         <f t="array" ref="C149">XLOOKUP(A149,Kits!$C:$C,Kits!$E:$E)</f>
         <v>2025210BLEFA</v>
       </c>
-      <c r="D149" s="18" t="str">
+      <c r="D149" s="19" t="str">
         <f t="array" ref="D149">XLOOKUP(A149,Kits!$C:$C,Kits!$F:$F)</f>
         <v>02/27</v>
       </c>
     </row>
     <row r="150" ht="14.25" customHeight="1">
-      <c r="A150" s="19" t="s">
+      <c r="A150" s="20" t="s">
         <v>430</v>
       </c>
-      <c r="B150" s="20" t="s">
+      <c r="B150" s="21" t="s">
         <v>431</v>
       </c>
-      <c r="C150" s="17" t="str">
+      <c r="C150" s="18" t="str">
         <f t="array" ref="C150">XLOOKUP(A150,Kits!$C:$C,Kits!$E:$E)</f>
         <v>20241609BLEFL</v>
       </c>
-      <c r="D150" s="18" t="str">
+      <c r="D150" s="19" t="str">
         <f t="array" ref="D150">XLOOKUP(A150,Kits!$C:$C,Kits!$F:$F)</f>
         <v>09/26</v>
       </c>
     </row>
     <row r="151" ht="14.25" customHeight="1">
-      <c r="A151" s="16" t="s">
+      <c r="A151" s="17" t="s">
         <v>432</v>
       </c>
-      <c r="B151" s="16" t="s">
+      <c r="B151" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="C151" s="17" t="str">
+      <c r="C151" s="18" t="str">
         <f t="array" ref="C151">XLOOKUP(A151,Kits!$C:$C,Kits!$E:$E)</f>
         <v>20252207BLEMA</v>
       </c>
-      <c r="D151" s="18" t="str">
+      <c r="D151" s="19" t="str">
         <f t="array" ref="D151">XLOOKUP(A151,Kits!$C:$C,Kits!$F:$F)</f>
         <v>07/27</v>
       </c>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="A152" s="16" t="s">
+      <c r="A152" s="17" t="s">
         <v>434</v>
       </c>
-      <c r="B152" s="16" t="s">
+      <c r="B152" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="C152" s="17" t="str">
+      <c r="C152" s="18" t="str">
         <f t="array" ref="C152">XLOOKUP(A152,Kits!$C:$C,Kits!$E:$E)</f>
         <v>20252602BLESR</v>
       </c>
-      <c r="D152" s="18" t="str">
+      <c r="D152" s="19" t="str">
         <f t="array" ref="D152">XLOOKUP(A152,Kits!$C:$C,Kits!$F:$F)</f>
         <v>02/27</v>
       </c>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="A153" s="16" t="s">
+      <c r="A153" s="17" t="s">
         <v>436</v>
       </c>
-      <c r="B153" s="16" t="s">
+      <c r="B153" s="17" t="s">
         <v>437</v>
       </c>
-      <c r="C153" s="17" t="str">
+      <c r="C153" s="18" t="str">
         <f t="array" ref="C153">XLOOKUP(A153,Kits!$C:$C,Kits!$E:$E)</f>
         <v>OLFA2508</v>
       </c>
-      <c r="D153" s="18" t="str">
+      <c r="D153" s="19" t="str">
         <f t="array" ref="D153">XLOOKUP(A153,Kits!$C:$C,Kits!$F:$F)</f>
         <v>08/27</v>
       </c>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="A154" s="16" t="s">
+      <c r="A154" s="17" t="s">
         <v>438</v>
       </c>
-      <c r="B154" s="16" t="s">
+      <c r="B154" s="17" t="s">
         <v>439</v>
       </c>
-      <c r="C154" s="17" t="str">
+      <c r="C154" s="18" t="str">
         <f t="array" ref="C154">XLOOKUP(A154,Kits!$C:$C,Kits!$E:$E)</f>
         <v>OLFL2510</v>
       </c>
-      <c r="D154" s="18" t="str">
+      <c r="D154" s="19" t="str">
         <f t="array" ref="D154">XLOOKUP(A154,Kits!$C:$C,Kits!$F:$F)</f>
         <v>10/27</v>
       </c>
     </row>
     <row r="155" ht="14.25" customHeight="1">
-      <c r="A155" s="16" t="s">
+      <c r="A155" s="17" t="s">
         <v>440</v>
       </c>
-      <c r="B155" s="16" t="s">
+      <c r="B155" s="17" t="s">
         <v>441</v>
       </c>
-      <c r="C155" s="17" t="str">
+      <c r="C155" s="18" t="str">
         <f t="array" ref="C155">XLOOKUP(A155,Kits!$C:$C,Kits!$E:$E)</f>
         <v>OLIN2508</v>
       </c>
-      <c r="D155" s="18" t="str">
+      <c r="D155" s="19" t="str">
         <f t="array" ref="D155">XLOOKUP(A155,Kits!$C:$C,Kits!$F:$F)</f>
         <v>08/27</v>
       </c>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="A156" s="16" t="s">
+      <c r="A156" s="17" t="s">
         <v>442</v>
       </c>
-      <c r="B156" s="16" t="s">
+      <c r="B156" s="17" t="s">
         <v>443</v>
       </c>
-      <c r="C156" s="17" t="str">
+      <c r="C156" s="18" t="str">
         <f t="array" ref="C156">XLOOKUP(A156,Kits!$C:$C,Kits!$E:$E)</f>
         <v>OLLA2507</v>
       </c>
-      <c r="D156" s="18" t="str">
+      <c r="D156" s="19" t="str">
         <f t="array" ref="D156">XLOOKUP(A156,Kits!$C:$C,Kits!$F:$F)</f>
         <v>07/27</v>
       </c>
     </row>
     <row r="157" ht="14.25" customHeight="1">
-      <c r="A157" s="16" t="s">
+      <c r="A157" s="17" t="s">
         <v>444</v>
       </c>
-      <c r="B157" s="16" t="s">
+      <c r="B157" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="C157" s="17" t="str">
+      <c r="C157" s="18" t="str">
         <f t="array" ref="C157">XLOOKUP(A157,Kits!$C:$C,Kits!$E:$E)</f>
         <v>OLMP2509</v>
       </c>
-      <c r="D157" s="18" t="str">
+      <c r="D157" s="19" t="str">
         <f t="array" ref="D157">XLOOKUP(A157,Kits!$C:$C,Kits!$F:$F)</f>
         <v>09/27</v>
       </c>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="A158" s="16" t="s">
+      <c r="A158" s="17" t="s">
         <v>446</v>
       </c>
-      <c r="B158" s="16" t="s">
+      <c r="B158" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="C158" s="17" t="str">
+      <c r="C158" s="18" t="str">
         <f t="array" ref="C158">XLOOKUP(A158,Kits!$C:$C,Kits!$E:$E)</f>
         <v>OLMC2509</v>
       </c>
-      <c r="D158" s="18" t="str">
+      <c r="D158" s="19" t="str">
         <f t="array" ref="D158">XLOOKUP(A158,Kits!$C:$C,Kits!$F:$F)</f>
         <v>09/27</v>
       </c>
     </row>
     <row r="159" ht="14.25" customHeight="1">
-      <c r="A159" s="16" t="s">
+      <c r="A159" s="17" t="s">
         <v>448</v>
       </c>
-      <c r="B159" s="16" t="s">
+      <c r="B159" s="17" t="s">
         <v>449</v>
       </c>
-      <c r="C159" s="17" t="str">
+      <c r="C159" s="18" t="str">
         <f t="array" ref="C159">XLOOKUP(A159,Kits!$C:$C,Kits!$E:$E)</f>
         <v>OLPV2510</v>
       </c>
-      <c r="D159" s="18" t="str">
+      <c r="D159" s="19" t="str">
         <f t="array" ref="D159">XLOOKUP(A159,Kits!$C:$C,Kits!$F:$F)</f>
         <v>10/27</v>
       </c>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="A160" s="16" t="s">
+      <c r="A160" s="17" t="s">
         <v>450</v>
       </c>
-      <c r="B160" s="16" t="s">
+      <c r="B160" s="17" t="s">
         <v>451</v>
       </c>
-      <c r="C160" s="17" t="str">
+      <c r="C160" s="18" t="str">
         <f t="array" ref="C160">XLOOKUP(A160,Kits!$C:$C,Kits!$E:$E)</f>
         <v>OLSR2508</v>
       </c>
-      <c r="D160" s="18" t="str">
+      <c r="D160" s="19" t="str">
         <f t="array" ref="D160">XLOOKUP(A160,Kits!$C:$C,Kits!$F:$F)</f>
         <v>08/27</v>
       </c>
@@ -6116,13 +6119,13 @@
       </c>
     </row>
     <row r="164" ht="14.25" customHeight="1">
-      <c r="A164" s="19" t="s">
+      <c r="A164" s="20" t="s">
         <v>462</v>
       </c>
-      <c r="B164" s="20" t="s">
+      <c r="B164" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="C164" s="19" t="s">
+      <c r="C164" s="20" t="s">
         <v>92</v>
       </c>
       <c r="D164" s="15" t="s">
@@ -6130,96 +6133,96 @@
       </c>
     </row>
     <row r="165" ht="14.25" customHeight="1">
-      <c r="A165" s="16" t="s">
+      <c r="A165" s="17" t="s">
         <v>464</v>
       </c>
-      <c r="B165" s="16" t="s">
+      <c r="B165" s="17" t="s">
         <v>465</v>
       </c>
-      <c r="C165" s="17" t="str">
+      <c r="C165" s="18" t="str">
         <f t="array" ref="C165">XLOOKUP(A165,Kits!$C:$C,Kits!$E:$E)</f>
         <v>2025210BLEFA</v>
       </c>
-      <c r="D165" s="18" t="str">
+      <c r="D165" s="19" t="str">
         <f t="array" ref="D165">XLOOKUP(A165,Kits!$C:$C,Kits!$F:$F)</f>
         <v>02/27</v>
       </c>
     </row>
     <row r="166" ht="14.25" customHeight="1">
-      <c r="A166" s="19" t="s">
+      <c r="A166" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B166" s="20" t="s">
+      <c r="B166" s="21" t="s">
         <v>467</v>
       </c>
-      <c r="C166" s="17" t="str">
+      <c r="C166" s="18" t="str">
         <f t="array" ref="C166">XLOOKUP(A166,Kits!$C:$C,Kits!$E:$E)</f>
         <v>20241609BLEFL</v>
       </c>
-      <c r="D166" s="18" t="str">
+      <c r="D166" s="19" t="str">
         <f t="array" ref="D166">XLOOKUP(A166,Kits!$C:$C,Kits!$F:$F)</f>
         <v>09/26</v>
       </c>
     </row>
     <row r="167" ht="14.25" customHeight="1">
-      <c r="A167" s="16" t="s">
+      <c r="A167" s="17" t="s">
         <v>468</v>
       </c>
-      <c r="B167" s="16" t="s">
+      <c r="B167" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="C167" s="17" t="str">
+      <c r="C167" s="18" t="str">
         <f t="array" ref="C167">XLOOKUP(A167,Kits!$C:$C,Kits!$E:$E)</f>
         <v>20252207BLEMA</v>
       </c>
-      <c r="D167" s="18" t="str">
+      <c r="D167" s="19" t="str">
         <f t="array" ref="D167">XLOOKUP(A167,Kits!$C:$C,Kits!$F:$F)</f>
         <v>07/27</v>
       </c>
     </row>
     <row r="168" ht="14.25" customHeight="1">
-      <c r="A168" s="16" t="s">
+      <c r="A168" s="17" t="s">
         <v>470</v>
       </c>
-      <c r="B168" s="16" t="s">
+      <c r="B168" s="17" t="s">
         <v>471</v>
       </c>
-      <c r="C168" s="17" t="str">
+      <c r="C168" s="18" t="str">
         <f t="array" ref="C168">XLOOKUP(A168,Kits!$C:$C,Kits!$E:$E)</f>
         <v>20252207BLEMA</v>
       </c>
-      <c r="D168" s="18" t="str">
+      <c r="D168" s="19" t="str">
         <f t="array" ref="D168">XLOOKUP(A168,Kits!$C:$C,Kits!$F:$F)</f>
         <v>07/27</v>
       </c>
     </row>
     <row r="169" ht="14.25" customHeight="1">
-      <c r="A169" s="16" t="s">
+      <c r="A169" s="17" t="s">
         <v>472</v>
       </c>
-      <c r="B169" s="16" t="s">
+      <c r="B169" s="17" t="s">
         <v>473</v>
       </c>
-      <c r="C169" s="21" t="s">
+      <c r="C169" s="22" t="s">
         <v>474</v>
       </c>
-      <c r="D169" s="18" t="str">
+      <c r="D169" s="19" t="str">
         <f t="array" ref="D169">XLOOKUP(A169,Kits!$C:$C,Kits!$F:$F)</f>
         <v>10/28</v>
       </c>
     </row>
     <row r="170" ht="14.25" customHeight="1">
-      <c r="A170" s="16" t="s">
+      <c r="A170" s="17" t="s">
         <v>475</v>
       </c>
-      <c r="B170" s="16" t="s">
+      <c r="B170" s="17" t="s">
         <v>476</v>
       </c>
-      <c r="C170" s="22" t="str">
+      <c r="C170" s="23" t="str">
         <f t="array" ref="C170">XLOOKUP(A170,Kits!$C:$C,Kits!$E:$E)</f>
         <v>J2304/J2267</v>
       </c>
-      <c r="D170" s="18" t="str">
+      <c r="D170" s="19" t="str">
         <f t="array" ref="D170">XLOOKUP(A170,Kits!$C:$C,Kits!$F:$F)</f>
         <v>10/28</v>
       </c>
@@ -6239,127 +6242,127 @@
       </c>
     </row>
     <row r="172" ht="14.25" customHeight="1">
-      <c r="A172" s="19" t="s">
+      <c r="A172" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="B172" s="20" t="s">
+      <c r="B172" s="21" t="s">
         <v>480</v>
       </c>
-      <c r="C172" s="17" t="str">
+      <c r="C172" s="18" t="str">
         <f t="array" ref="C172">XLOOKUP(A172,Kits!$C:$C,Kits!$E:$E)</f>
         <v>20240601BLEPE</v>
       </c>
-      <c r="D172" s="18" t="str">
+      <c r="D172" s="19" t="str">
         <f t="array" ref="D172">XLOOKUP(A172,Kits!$C:$C,Kits!$F:$F)</f>
         <v>06/26</v>
       </c>
     </row>
     <row r="173" ht="14.25" customHeight="1">
-      <c r="A173" s="16" t="s">
+      <c r="A173" s="17" t="s">
         <v>481</v>
       </c>
-      <c r="B173" s="16" t="s">
+      <c r="B173" s="17" t="s">
         <v>482</v>
       </c>
-      <c r="C173" s="17" t="str">
+      <c r="C173" s="18" t="str">
         <f t="array" ref="C173">XLOOKUP(A173,Kits!$C:$C,Kits!$E:$E)</f>
         <v>240105</v>
       </c>
-      <c r="D173" s="18" t="str">
+      <c r="D173" s="19" t="str">
         <f t="array" ref="D173">XLOOKUP(A173,Kits!$C:$C,Kits!$F:$F)</f>
         <v>11/27</v>
       </c>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="A174" s="16" t="s">
+      <c r="A174" s="17" t="s">
         <v>483</v>
       </c>
-      <c r="B174" s="16" t="s">
+      <c r="B174" s="17" t="s">
         <v>484</v>
       </c>
-      <c r="C174" s="21" t="s">
+      <c r="C174" s="22" t="s">
         <v>485</v>
       </c>
-      <c r="D174" s="23" t="s">
+      <c r="D174" s="24" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="175" ht="14.25" customHeight="1">
-      <c r="A175" s="16" t="s">
+      <c r="A175" s="17" t="s">
         <v>486</v>
       </c>
-      <c r="B175" s="16" t="s">
+      <c r="B175" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="C175" s="17" t="str">
+      <c r="C175" s="18" t="str">
         <f t="array" ref="C175">XLOOKUP(A175,Kits!$C:$C,Kits!$E:$E)</f>
         <v>240205</v>
       </c>
-      <c r="D175" s="18" t="str">
+      <c r="D175" s="19" t="str">
         <f t="array" ref="D175">XLOOKUP(A175,Kits!$C:$C,Kits!$F:$F)</f>
         <v>10/27</v>
       </c>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="A176" s="16" t="s">
+      <c r="A176" s="17" t="s">
         <v>488</v>
       </c>
-      <c r="B176" s="16" t="s">
+      <c r="B176" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="C176" s="17" t="str">
+      <c r="C176" s="18" t="str">
         <f t="array" ref="C176">XLOOKUP(A176,Kits!$C:$C,Kits!$E:$E)</f>
         <v>240204</v>
       </c>
-      <c r="D176" s="18" t="str">
+      <c r="D176" s="19" t="str">
         <f t="array" ref="D176">XLOOKUP(A176,Kits!$C:$C,Kits!$F:$F)</f>
         <v>09/27</v>
       </c>
     </row>
     <row r="177" ht="14.25" customHeight="1">
-      <c r="A177" s="24" t="s">
+      <c r="A177" s="25" t="s">
         <v>490</v>
       </c>
-      <c r="B177" s="16" t="s">
+      <c r="B177" s="17" t="s">
         <v>491</v>
       </c>
-      <c r="C177" s="17" t="str">
+      <c r="C177" s="18" t="str">
         <f t="array" ref="C177">XLOOKUP(A177,Kits!$C:$C,Kits!$E:$E)</f>
         <v>240303</v>
       </c>
-      <c r="D177" s="18" t="str">
+      <c r="D177" s="19" t="str">
         <f t="array" ref="D177">XLOOKUP(A177,Kits!$C:$C,Kits!$F:$F)</f>
         <v>08/28</v>
       </c>
     </row>
     <row r="178" ht="14.25" customHeight="1">
-      <c r="A178" s="16" t="s">
+      <c r="A178" s="17" t="s">
         <v>492</v>
       </c>
-      <c r="B178" s="16" t="s">
+      <c r="B178" s="17" t="s">
         <v>493</v>
       </c>
-      <c r="C178" s="17" t="str">
+      <c r="C178" s="18" t="str">
         <f t="array" ref="C178">XLOOKUP(A178,Kits!$C:$C,Kits!$E:$E)</f>
         <v>250302</v>
       </c>
-      <c r="D178" s="18" t="str">
+      <c r="D178" s="19" t="str">
         <f t="array" ref="D178">XLOOKUP(A178,Kits!$C:$C,Kits!$F:$F)</f>
         <v>07/28</v>
       </c>
     </row>
     <row r="179" ht="14.25" customHeight="1">
-      <c r="A179" s="16" t="s">
+      <c r="A179" s="17" t="s">
         <v>494</v>
       </c>
-      <c r="B179" s="16" t="s">
+      <c r="B179" s="17" t="s">
         <v>495</v>
       </c>
-      <c r="C179" s="17" t="str">
+      <c r="C179" s="18" t="str">
         <f t="array" ref="C179">XLOOKUP(A179,Kits!$C:$C,Kits!$E:$E)</f>
         <v>LEN89.0005</v>
       </c>
-      <c r="D179" s="18" t="str">
+      <c r="D179" s="19" t="str">
         <f t="array" ref="D179">XLOOKUP(A179,Kits!$C:$C,Kits!$F:$F)</f>
         <v>10/28</v>
       </c>
@@ -6371,7 +6374,7 @@
       <c r="B180" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="C180" s="11" t="s">
+      <c r="C180" s="16" t="s">
         <v>498</v>
       </c>
       <c r="D180" s="8" t="s">
@@ -6379,17 +6382,17 @@
       </c>
     </row>
     <row r="181" ht="14.25" customHeight="1">
-      <c r="A181" s="16" t="s">
+      <c r="A181" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="B181" s="16" t="s">
+      <c r="B181" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="C181" s="17" t="str">
+      <c r="C181" s="18" t="str">
         <f t="array" ref="C181">XLOOKUP(A181,Kits!$C:$C,Kits!$E:$E)</f>
         <v>20252602BLESR</v>
       </c>
-      <c r="D181" s="18" t="str">
+      <c r="D181" s="19" t="str">
         <f t="array" ref="D181">XLOOKUP(A181,Kits!$C:$C,Kits!$F:$F)</f>
         <v>02/27</v>
       </c>
@@ -6534,7 +6537,7 @@
       <c r="A192" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="B192" s="25" t="s">
+      <c r="B192" s="26" t="s">
         <v>532</v>
       </c>
       <c r="C192" s="7" t="s">
@@ -7685,7 +7688,7 @@
       <c r="B274" s="6" t="s">
         <v>765</v>
       </c>
-      <c r="C274" s="11" t="s">
+      <c r="C274" s="16" t="s">
         <v>766</v>
       </c>
       <c r="D274" s="8" t="s">
@@ -8581,7 +8584,7 @@
       <c r="B338" s="6" t="s">
         <v>939</v>
       </c>
-      <c r="C338" s="26" t="s">
+      <c r="C338" s="27" t="s">
         <v>940</v>
       </c>
       <c r="D338" s="8" t="s">
@@ -9354,7 +9357,7 @@
       <c r="A394" s="7" t="s">
         <v>1093</v>
       </c>
-      <c r="B394" s="27" t="s">
+      <c r="B394" s="28" t="s">
         <v>1094</v>
       </c>
       <c r="C394" s="7" t="s">
@@ -9368,7 +9371,7 @@
       <c r="A395" s="7" t="s">
         <v>1096</v>
       </c>
-      <c r="B395" s="28" t="s">
+      <c r="B395" s="29" t="s">
         <v>1097</v>
       </c>
       <c r="C395" s="7" t="s">
@@ -9379,1204 +9382,1204 @@
       </c>
     </row>
     <row r="396" ht="14.25" customHeight="1">
-      <c r="A396" s="29"/>
-      <c r="B396" s="27"/>
-      <c r="C396" s="29"/>
-      <c r="D396" s="29"/>
+      <c r="A396" s="30"/>
+      <c r="B396" s="28"/>
+      <c r="C396" s="30"/>
+      <c r="D396" s="30"/>
     </row>
     <row r="397" ht="14.25" customHeight="1">
-      <c r="A397" s="29"/>
-      <c r="B397" s="27"/>
-      <c r="C397" s="29"/>
-      <c r="D397" s="29"/>
+      <c r="A397" s="30"/>
+      <c r="B397" s="28"/>
+      <c r="C397" s="30"/>
+      <c r="D397" s="30"/>
     </row>
     <row r="398" ht="14.25" customHeight="1">
-      <c r="A398" s="29"/>
-      <c r="B398" s="27"/>
-      <c r="C398" s="29"/>
-      <c r="D398" s="29"/>
+      <c r="A398" s="30"/>
+      <c r="B398" s="28"/>
+      <c r="C398" s="30"/>
+      <c r="D398" s="30"/>
     </row>
     <row r="399" ht="14.25" customHeight="1">
-      <c r="A399" s="29"/>
-      <c r="B399" s="27"/>
-      <c r="C399" s="29"/>
-      <c r="D399" s="29"/>
+      <c r="A399" s="30"/>
+      <c r="B399" s="28"/>
+      <c r="C399" s="30"/>
+      <c r="D399" s="30"/>
     </row>
     <row r="400" ht="14.25" customHeight="1">
-      <c r="A400" s="30"/>
-      <c r="B400" s="31"/>
-      <c r="C400" s="30"/>
-      <c r="D400" s="30"/>
+      <c r="A400" s="31"/>
+      <c r="B400" s="32"/>
+      <c r="C400" s="31"/>
+      <c r="D400" s="31"/>
     </row>
     <row r="401" ht="14.25" customHeight="1">
-      <c r="A401" s="30"/>
-      <c r="B401" s="31"/>
-      <c r="C401" s="30"/>
-      <c r="D401" s="30"/>
+      <c r="A401" s="31"/>
+      <c r="B401" s="32"/>
+      <c r="C401" s="31"/>
+      <c r="D401" s="31"/>
     </row>
     <row r="402" ht="14.25" customHeight="1">
-      <c r="A402" s="30"/>
-      <c r="B402" s="31"/>
-      <c r="C402" s="30"/>
-      <c r="D402" s="30"/>
+      <c r="A402" s="31"/>
+      <c r="B402" s="32"/>
+      <c r="C402" s="31"/>
+      <c r="D402" s="31"/>
     </row>
     <row r="403" ht="14.25" customHeight="1">
-      <c r="A403" s="30"/>
-      <c r="B403" s="31"/>
-      <c r="C403" s="30"/>
-      <c r="D403" s="30"/>
+      <c r="A403" s="31"/>
+      <c r="B403" s="32"/>
+      <c r="C403" s="31"/>
+      <c r="D403" s="31"/>
     </row>
     <row r="404" ht="14.25" customHeight="1">
-      <c r="A404" s="30"/>
-      <c r="B404" s="31"/>
-      <c r="C404" s="30"/>
-      <c r="D404" s="30"/>
+      <c r="A404" s="31"/>
+      <c r="B404" s="32"/>
+      <c r="C404" s="31"/>
+      <c r="D404" s="31"/>
     </row>
     <row r="405" ht="14.25" customHeight="1">
-      <c r="A405" s="30"/>
-      <c r="B405" s="31"/>
-      <c r="C405" s="30"/>
-      <c r="D405" s="30"/>
+      <c r="A405" s="31"/>
+      <c r="B405" s="32"/>
+      <c r="C405" s="31"/>
+      <c r="D405" s="31"/>
     </row>
     <row r="406" ht="14.25" customHeight="1">
-      <c r="A406" s="30"/>
-      <c r="B406" s="31"/>
-      <c r="C406" s="30"/>
-      <c r="D406" s="30"/>
+      <c r="A406" s="31"/>
+      <c r="B406" s="32"/>
+      <c r="C406" s="31"/>
+      <c r="D406" s="31"/>
     </row>
     <row r="407" ht="14.25" customHeight="1">
-      <c r="A407" s="30"/>
-      <c r="B407" s="31"/>
-      <c r="C407" s="30"/>
-      <c r="D407" s="30"/>
+      <c r="A407" s="31"/>
+      <c r="B407" s="32"/>
+      <c r="C407" s="31"/>
+      <c r="D407" s="31"/>
     </row>
     <row r="408" ht="14.25" customHeight="1">
-      <c r="A408" s="30"/>
-      <c r="B408" s="31"/>
-      <c r="C408" s="30"/>
-      <c r="D408" s="30"/>
+      <c r="A408" s="31"/>
+      <c r="B408" s="32"/>
+      <c r="C408" s="31"/>
+      <c r="D408" s="31"/>
     </row>
     <row r="409" ht="14.25" customHeight="1">
-      <c r="A409" s="30"/>
-      <c r="B409" s="31"/>
-      <c r="C409" s="30"/>
-      <c r="D409" s="30"/>
+      <c r="A409" s="31"/>
+      <c r="B409" s="32"/>
+      <c r="C409" s="31"/>
+      <c r="D409" s="31"/>
     </row>
     <row r="410" ht="14.25" customHeight="1">
-      <c r="A410" s="30"/>
-      <c r="B410" s="31"/>
-      <c r="C410" s="30"/>
-      <c r="D410" s="30"/>
+      <c r="A410" s="31"/>
+      <c r="B410" s="32"/>
+      <c r="C410" s="31"/>
+      <c r="D410" s="31"/>
     </row>
     <row r="411" ht="14.25" customHeight="1">
-      <c r="A411" s="30"/>
-      <c r="B411" s="31"/>
-      <c r="C411" s="30"/>
-      <c r="D411" s="30"/>
+      <c r="A411" s="31"/>
+      <c r="B411" s="32"/>
+      <c r="C411" s="31"/>
+      <c r="D411" s="31"/>
     </row>
     <row r="412" ht="14.25" customHeight="1">
-      <c r="A412" s="30"/>
-      <c r="B412" s="31"/>
-      <c r="C412" s="30"/>
-      <c r="D412" s="30"/>
+      <c r="A412" s="31"/>
+      <c r="B412" s="32"/>
+      <c r="C412" s="31"/>
+      <c r="D412" s="31"/>
     </row>
     <row r="413" ht="14.25" customHeight="1">
-      <c r="A413" s="30"/>
-      <c r="B413" s="31"/>
-      <c r="C413" s="30"/>
-      <c r="D413" s="30"/>
+      <c r="A413" s="31"/>
+      <c r="B413" s="32"/>
+      <c r="C413" s="31"/>
+      <c r="D413" s="31"/>
     </row>
     <row r="414" ht="14.25" customHeight="1">
-      <c r="A414" s="30"/>
-      <c r="B414" s="31"/>
-      <c r="C414" s="30"/>
-      <c r="D414" s="30"/>
+      <c r="A414" s="31"/>
+      <c r="B414" s="32"/>
+      <c r="C414" s="31"/>
+      <c r="D414" s="31"/>
     </row>
     <row r="415" ht="14.25" customHeight="1">
-      <c r="A415" s="30"/>
-      <c r="B415" s="31"/>
-      <c r="C415" s="30"/>
-      <c r="D415" s="30"/>
+      <c r="A415" s="31"/>
+      <c r="B415" s="32"/>
+      <c r="C415" s="31"/>
+      <c r="D415" s="31"/>
     </row>
     <row r="416" ht="14.25" customHeight="1">
-      <c r="A416" s="30"/>
-      <c r="B416" s="31"/>
-      <c r="C416" s="30"/>
-      <c r="D416" s="30"/>
+      <c r="A416" s="31"/>
+      <c r="B416" s="32"/>
+      <c r="C416" s="31"/>
+      <c r="D416" s="31"/>
     </row>
     <row r="417" ht="14.25" customHeight="1">
-      <c r="A417" s="30"/>
-      <c r="B417" s="31"/>
-      <c r="C417" s="30"/>
-      <c r="D417" s="30"/>
+      <c r="A417" s="31"/>
+      <c r="B417" s="32"/>
+      <c r="C417" s="31"/>
+      <c r="D417" s="31"/>
     </row>
     <row r="418" ht="14.25" customHeight="1">
-      <c r="A418" s="30"/>
-      <c r="B418" s="31"/>
-      <c r="C418" s="30"/>
-      <c r="D418" s="30"/>
+      <c r="A418" s="31"/>
+      <c r="B418" s="32"/>
+      <c r="C418" s="31"/>
+      <c r="D418" s="31"/>
     </row>
     <row r="419" ht="14.25" customHeight="1">
-      <c r="A419" s="30"/>
-      <c r="B419" s="31"/>
-      <c r="C419" s="30"/>
-      <c r="D419" s="30"/>
+      <c r="A419" s="31"/>
+      <c r="B419" s="32"/>
+      <c r="C419" s="31"/>
+      <c r="D419" s="31"/>
     </row>
     <row r="420" ht="14.25" customHeight="1">
-      <c r="A420" s="30"/>
-      <c r="B420" s="31"/>
-      <c r="C420" s="30"/>
-      <c r="D420" s="30"/>
+      <c r="A420" s="31"/>
+      <c r="B420" s="32"/>
+      <c r="C420" s="31"/>
+      <c r="D420" s="31"/>
     </row>
     <row r="421" ht="14.25" customHeight="1">
-      <c r="A421" s="30"/>
-      <c r="B421" s="31"/>
-      <c r="C421" s="30"/>
-      <c r="D421" s="30"/>
+      <c r="A421" s="31"/>
+      <c r="B421" s="32"/>
+      <c r="C421" s="31"/>
+      <c r="D421" s="31"/>
     </row>
     <row r="422" ht="14.25" customHeight="1">
-      <c r="A422" s="30"/>
-      <c r="B422" s="31"/>
-      <c r="C422" s="30"/>
-      <c r="D422" s="30"/>
+      <c r="A422" s="31"/>
+      <c r="B422" s="32"/>
+      <c r="C422" s="31"/>
+      <c r="D422" s="31"/>
     </row>
     <row r="423" ht="14.25" customHeight="1">
-      <c r="A423" s="30"/>
-      <c r="B423" s="31"/>
-      <c r="C423" s="30"/>
-      <c r="D423" s="30"/>
+      <c r="A423" s="31"/>
+      <c r="B423" s="32"/>
+      <c r="C423" s="31"/>
+      <c r="D423" s="31"/>
     </row>
     <row r="424" ht="14.25" customHeight="1">
-      <c r="A424" s="30"/>
-      <c r="B424" s="31"/>
-      <c r="C424" s="30"/>
-      <c r="D424" s="30"/>
+      <c r="A424" s="31"/>
+      <c r="B424" s="32"/>
+      <c r="C424" s="31"/>
+      <c r="D424" s="31"/>
     </row>
     <row r="425" ht="14.25" customHeight="1">
-      <c r="A425" s="30"/>
-      <c r="B425" s="31"/>
-      <c r="C425" s="30"/>
-      <c r="D425" s="30"/>
+      <c r="A425" s="31"/>
+      <c r="B425" s="32"/>
+      <c r="C425" s="31"/>
+      <c r="D425" s="31"/>
     </row>
     <row r="426" ht="14.25" customHeight="1">
-      <c r="A426" s="30"/>
-      <c r="B426" s="31"/>
-      <c r="C426" s="30"/>
-      <c r="D426" s="30"/>
+      <c r="A426" s="31"/>
+      <c r="B426" s="32"/>
+      <c r="C426" s="31"/>
+      <c r="D426" s="31"/>
     </row>
     <row r="427" ht="14.25" customHeight="1">
-      <c r="A427" s="30"/>
-      <c r="B427" s="31"/>
-      <c r="C427" s="30"/>
-      <c r="D427" s="30"/>
+      <c r="A427" s="31"/>
+      <c r="B427" s="32"/>
+      <c r="C427" s="31"/>
+      <c r="D427" s="31"/>
     </row>
     <row r="428" ht="14.25" customHeight="1">
-      <c r="A428" s="30"/>
-      <c r="B428" s="31"/>
-      <c r="C428" s="30"/>
-      <c r="D428" s="30"/>
+      <c r="A428" s="31"/>
+      <c r="B428" s="32"/>
+      <c r="C428" s="31"/>
+      <c r="D428" s="31"/>
     </row>
     <row r="429" ht="14.25" customHeight="1">
-      <c r="A429" s="30"/>
-      <c r="B429" s="31"/>
-      <c r="C429" s="30"/>
-      <c r="D429" s="30"/>
+      <c r="A429" s="31"/>
+      <c r="B429" s="32"/>
+      <c r="C429" s="31"/>
+      <c r="D429" s="31"/>
     </row>
     <row r="430" ht="14.25" customHeight="1">
-      <c r="A430" s="30"/>
-      <c r="B430" s="31"/>
-      <c r="C430" s="30"/>
-      <c r="D430" s="30"/>
+      <c r="A430" s="31"/>
+      <c r="B430" s="32"/>
+      <c r="C430" s="31"/>
+      <c r="D430" s="31"/>
     </row>
     <row r="431" ht="14.25" customHeight="1">
-      <c r="A431" s="30"/>
-      <c r="B431" s="31"/>
-      <c r="C431" s="30"/>
-      <c r="D431" s="30"/>
+      <c r="A431" s="31"/>
+      <c r="B431" s="32"/>
+      <c r="C431" s="31"/>
+      <c r="D431" s="31"/>
     </row>
     <row r="432" ht="14.25" customHeight="1">
-      <c r="A432" s="30"/>
-      <c r="B432" s="31"/>
-      <c r="C432" s="30"/>
-      <c r="D432" s="30"/>
+      <c r="A432" s="31"/>
+      <c r="B432" s="32"/>
+      <c r="C432" s="31"/>
+      <c r="D432" s="31"/>
     </row>
     <row r="433" ht="14.25" customHeight="1">
-      <c r="A433" s="30"/>
-      <c r="B433" s="31"/>
-      <c r="C433" s="30"/>
-      <c r="D433" s="30"/>
+      <c r="A433" s="31"/>
+      <c r="B433" s="32"/>
+      <c r="C433" s="31"/>
+      <c r="D433" s="31"/>
     </row>
     <row r="434" ht="14.25" customHeight="1">
-      <c r="A434" s="30"/>
-      <c r="B434" s="31"/>
-      <c r="C434" s="30"/>
-      <c r="D434" s="30"/>
+      <c r="A434" s="31"/>
+      <c r="B434" s="32"/>
+      <c r="C434" s="31"/>
+      <c r="D434" s="31"/>
     </row>
     <row r="435" ht="14.25" customHeight="1">
-      <c r="A435" s="30"/>
-      <c r="B435" s="31"/>
-      <c r="C435" s="30"/>
-      <c r="D435" s="30"/>
+      <c r="A435" s="31"/>
+      <c r="B435" s="32"/>
+      <c r="C435" s="31"/>
+      <c r="D435" s="31"/>
     </row>
     <row r="436" ht="14.25" customHeight="1">
-      <c r="A436" s="30"/>
-      <c r="B436" s="31"/>
-      <c r="C436" s="30"/>
-      <c r="D436" s="30"/>
+      <c r="A436" s="31"/>
+      <c r="B436" s="32"/>
+      <c r="C436" s="31"/>
+      <c r="D436" s="31"/>
     </row>
     <row r="437" ht="14.25" customHeight="1">
-      <c r="A437" s="30"/>
-      <c r="B437" s="31"/>
-      <c r="C437" s="30"/>
-      <c r="D437" s="30"/>
+      <c r="A437" s="31"/>
+      <c r="B437" s="32"/>
+      <c r="C437" s="31"/>
+      <c r="D437" s="31"/>
     </row>
     <row r="438" ht="14.25" customHeight="1">
-      <c r="A438" s="30"/>
-      <c r="B438" s="31"/>
-      <c r="C438" s="30"/>
-      <c r="D438" s="30"/>
+      <c r="A438" s="31"/>
+      <c r="B438" s="32"/>
+      <c r="C438" s="31"/>
+      <c r="D438" s="31"/>
     </row>
     <row r="439" ht="14.25" customHeight="1">
-      <c r="A439" s="30"/>
-      <c r="B439" s="31"/>
-      <c r="C439" s="30"/>
-      <c r="D439" s="30"/>
+      <c r="A439" s="31"/>
+      <c r="B439" s="32"/>
+      <c r="C439" s="31"/>
+      <c r="D439" s="31"/>
     </row>
     <row r="440" ht="14.25" customHeight="1">
-      <c r="A440" s="30"/>
-      <c r="B440" s="31"/>
-      <c r="C440" s="30"/>
-      <c r="D440" s="30"/>
+      <c r="A440" s="31"/>
+      <c r="B440" s="32"/>
+      <c r="C440" s="31"/>
+      <c r="D440" s="31"/>
     </row>
     <row r="441" ht="14.25" customHeight="1">
-      <c r="A441" s="30"/>
-      <c r="B441" s="31"/>
-      <c r="C441" s="30"/>
-      <c r="D441" s="30"/>
+      <c r="A441" s="31"/>
+      <c r="B441" s="32"/>
+      <c r="C441" s="31"/>
+      <c r="D441" s="31"/>
     </row>
     <row r="442" ht="14.25" customHeight="1">
-      <c r="A442" s="30"/>
-      <c r="B442" s="31"/>
-      <c r="C442" s="30"/>
-      <c r="D442" s="30"/>
+      <c r="A442" s="31"/>
+      <c r="B442" s="32"/>
+      <c r="C442" s="31"/>
+      <c r="D442" s="31"/>
     </row>
     <row r="443" ht="14.25" customHeight="1">
-      <c r="A443" s="30"/>
-      <c r="B443" s="31"/>
-      <c r="C443" s="30"/>
-      <c r="D443" s="30"/>
+      <c r="A443" s="31"/>
+      <c r="B443" s="32"/>
+      <c r="C443" s="31"/>
+      <c r="D443" s="31"/>
     </row>
     <row r="444" ht="14.25" customHeight="1">
-      <c r="A444" s="30"/>
-      <c r="B444" s="31"/>
-      <c r="C444" s="30"/>
-      <c r="D444" s="30"/>
+      <c r="A444" s="31"/>
+      <c r="B444" s="32"/>
+      <c r="C444" s="31"/>
+      <c r="D444" s="31"/>
     </row>
     <row r="445" ht="14.25" customHeight="1">
-      <c r="A445" s="30"/>
-      <c r="B445" s="31"/>
-      <c r="C445" s="30"/>
-      <c r="D445" s="30"/>
+      <c r="A445" s="31"/>
+      <c r="B445" s="32"/>
+      <c r="C445" s="31"/>
+      <c r="D445" s="31"/>
     </row>
     <row r="446" ht="14.25" customHeight="1">
-      <c r="A446" s="30"/>
-      <c r="B446" s="31"/>
-      <c r="C446" s="30"/>
-      <c r="D446" s="30"/>
+      <c r="A446" s="31"/>
+      <c r="B446" s="32"/>
+      <c r="C446" s="31"/>
+      <c r="D446" s="31"/>
     </row>
     <row r="447" ht="14.25" customHeight="1">
-      <c r="A447" s="30"/>
-      <c r="B447" s="31"/>
-      <c r="C447" s="30"/>
-      <c r="D447" s="30"/>
+      <c r="A447" s="31"/>
+      <c r="B447" s="32"/>
+      <c r="C447" s="31"/>
+      <c r="D447" s="31"/>
     </row>
     <row r="448" ht="14.25" customHeight="1">
-      <c r="A448" s="30"/>
-      <c r="B448" s="31"/>
-      <c r="C448" s="30"/>
-      <c r="D448" s="30"/>
+      <c r="A448" s="31"/>
+      <c r="B448" s="32"/>
+      <c r="C448" s="31"/>
+      <c r="D448" s="31"/>
     </row>
     <row r="449" ht="14.25" customHeight="1">
-      <c r="A449" s="30"/>
-      <c r="B449" s="31"/>
-      <c r="C449" s="30"/>
-      <c r="D449" s="30"/>
+      <c r="A449" s="31"/>
+      <c r="B449" s="32"/>
+      <c r="C449" s="31"/>
+      <c r="D449" s="31"/>
     </row>
     <row r="450" ht="14.25" customHeight="1">
-      <c r="A450" s="30"/>
-      <c r="B450" s="31"/>
-      <c r="C450" s="30"/>
-      <c r="D450" s="30"/>
+      <c r="A450" s="31"/>
+      <c r="B450" s="32"/>
+      <c r="C450" s="31"/>
+      <c r="D450" s="31"/>
     </row>
     <row r="451" ht="14.25" customHeight="1">
-      <c r="A451" s="30"/>
-      <c r="B451" s="31"/>
-      <c r="C451" s="30"/>
-      <c r="D451" s="30"/>
+      <c r="A451" s="31"/>
+      <c r="B451" s="32"/>
+      <c r="C451" s="31"/>
+      <c r="D451" s="31"/>
     </row>
     <row r="452" ht="14.25" customHeight="1">
-      <c r="A452" s="30"/>
-      <c r="B452" s="31"/>
-      <c r="C452" s="30"/>
-      <c r="D452" s="30"/>
+      <c r="A452" s="31"/>
+      <c r="B452" s="32"/>
+      <c r="C452" s="31"/>
+      <c r="D452" s="31"/>
     </row>
     <row r="453" ht="14.25" customHeight="1">
-      <c r="A453" s="30"/>
-      <c r="B453" s="31"/>
-      <c r="C453" s="30"/>
-      <c r="D453" s="30"/>
+      <c r="A453" s="31"/>
+      <c r="B453" s="32"/>
+      <c r="C453" s="31"/>
+      <c r="D453" s="31"/>
     </row>
     <row r="454" ht="14.25" customHeight="1">
-      <c r="A454" s="30"/>
-      <c r="B454" s="31"/>
-      <c r="C454" s="30"/>
-      <c r="D454" s="30"/>
+      <c r="A454" s="31"/>
+      <c r="B454" s="32"/>
+      <c r="C454" s="31"/>
+      <c r="D454" s="31"/>
     </row>
     <row r="455" ht="14.25" customHeight="1">
-      <c r="A455" s="30"/>
-      <c r="B455" s="31"/>
-      <c r="C455" s="30"/>
-      <c r="D455" s="30"/>
+      <c r="A455" s="31"/>
+      <c r="B455" s="32"/>
+      <c r="C455" s="31"/>
+      <c r="D455" s="31"/>
     </row>
     <row r="456" ht="14.25" customHeight="1">
-      <c r="A456" s="30"/>
-      <c r="B456" s="31"/>
-      <c r="C456" s="30"/>
-      <c r="D456" s="30"/>
+      <c r="A456" s="31"/>
+      <c r="B456" s="32"/>
+      <c r="C456" s="31"/>
+      <c r="D456" s="31"/>
     </row>
     <row r="457" ht="14.25" customHeight="1">
-      <c r="A457" s="30"/>
-      <c r="B457" s="31"/>
-      <c r="C457" s="30"/>
-      <c r="D457" s="30"/>
+      <c r="A457" s="31"/>
+      <c r="B457" s="32"/>
+      <c r="C457" s="31"/>
+      <c r="D457" s="31"/>
     </row>
     <row r="458" ht="14.25" customHeight="1">
-      <c r="A458" s="30"/>
-      <c r="B458" s="31"/>
-      <c r="C458" s="30"/>
-      <c r="D458" s="30"/>
+      <c r="A458" s="31"/>
+      <c r="B458" s="32"/>
+      <c r="C458" s="31"/>
+      <c r="D458" s="31"/>
     </row>
     <row r="459" ht="14.25" customHeight="1">
-      <c r="A459" s="30"/>
-      <c r="B459" s="31"/>
-      <c r="C459" s="30"/>
-      <c r="D459" s="30"/>
+      <c r="A459" s="31"/>
+      <c r="B459" s="32"/>
+      <c r="C459" s="31"/>
+      <c r="D459" s="31"/>
     </row>
     <row r="460" ht="14.25" customHeight="1">
-      <c r="A460" s="30"/>
-      <c r="B460" s="31"/>
-      <c r="C460" s="30"/>
-      <c r="D460" s="30"/>
+      <c r="A460" s="31"/>
+      <c r="B460" s="32"/>
+      <c r="C460" s="31"/>
+      <c r="D460" s="31"/>
     </row>
     <row r="461" ht="14.25" customHeight="1">
-      <c r="A461" s="30"/>
-      <c r="B461" s="31"/>
-      <c r="C461" s="30"/>
-      <c r="D461" s="30"/>
+      <c r="A461" s="31"/>
+      <c r="B461" s="32"/>
+      <c r="C461" s="31"/>
+      <c r="D461" s="31"/>
     </row>
     <row r="462" ht="14.25" customHeight="1">
-      <c r="A462" s="30"/>
-      <c r="B462" s="31"/>
-      <c r="C462" s="30"/>
-      <c r="D462" s="30"/>
+      <c r="A462" s="31"/>
+      <c r="B462" s="32"/>
+      <c r="C462" s="31"/>
+      <c r="D462" s="31"/>
     </row>
     <row r="463" ht="14.25" customHeight="1">
-      <c r="A463" s="30"/>
-      <c r="B463" s="31"/>
-      <c r="C463" s="30"/>
-      <c r="D463" s="30"/>
+      <c r="A463" s="31"/>
+      <c r="B463" s="32"/>
+      <c r="C463" s="31"/>
+      <c r="D463" s="31"/>
     </row>
     <row r="464" ht="14.25" customHeight="1">
-      <c r="A464" s="30"/>
-      <c r="B464" s="31"/>
-      <c r="C464" s="30"/>
-      <c r="D464" s="30"/>
+      <c r="A464" s="31"/>
+      <c r="B464" s="32"/>
+      <c r="C464" s="31"/>
+      <c r="D464" s="31"/>
     </row>
     <row r="465" ht="14.25" customHeight="1">
-      <c r="A465" s="30"/>
-      <c r="B465" s="31"/>
-      <c r="C465" s="30"/>
-      <c r="D465" s="30"/>
+      <c r="A465" s="31"/>
+      <c r="B465" s="32"/>
+      <c r="C465" s="31"/>
+      <c r="D465" s="31"/>
     </row>
     <row r="466" ht="14.25" customHeight="1">
-      <c r="A466" s="30"/>
-      <c r="B466" s="31"/>
-      <c r="C466" s="30"/>
-      <c r="D466" s="30"/>
+      <c r="A466" s="31"/>
+      <c r="B466" s="32"/>
+      <c r="C466" s="31"/>
+      <c r="D466" s="31"/>
     </row>
     <row r="467" ht="14.25" customHeight="1">
-      <c r="A467" s="30"/>
-      <c r="B467" s="31"/>
-      <c r="C467" s="30"/>
-      <c r="D467" s="30"/>
+      <c r="A467" s="31"/>
+      <c r="B467" s="32"/>
+      <c r="C467" s="31"/>
+      <c r="D467" s="31"/>
     </row>
     <row r="468" ht="14.25" customHeight="1">
-      <c r="A468" s="30"/>
-      <c r="B468" s="31"/>
-      <c r="C468" s="30"/>
-      <c r="D468" s="30"/>
+      <c r="A468" s="31"/>
+      <c r="B468" s="32"/>
+      <c r="C468" s="31"/>
+      <c r="D468" s="31"/>
     </row>
     <row r="469" ht="14.25" customHeight="1">
-      <c r="A469" s="30"/>
-      <c r="B469" s="31"/>
-      <c r="C469" s="30"/>
-      <c r="D469" s="30"/>
+      <c r="A469" s="31"/>
+      <c r="B469" s="32"/>
+      <c r="C469" s="31"/>
+      <c r="D469" s="31"/>
     </row>
     <row r="470" ht="14.25" customHeight="1">
-      <c r="A470" s="30"/>
-      <c r="B470" s="31"/>
-      <c r="C470" s="30"/>
-      <c r="D470" s="30"/>
+      <c r="A470" s="31"/>
+      <c r="B470" s="32"/>
+      <c r="C470" s="31"/>
+      <c r="D470" s="31"/>
     </row>
     <row r="471" ht="14.25" customHeight="1">
-      <c r="A471" s="30"/>
-      <c r="B471" s="31"/>
-      <c r="C471" s="30"/>
-      <c r="D471" s="30"/>
+      <c r="A471" s="31"/>
+      <c r="B471" s="32"/>
+      <c r="C471" s="31"/>
+      <c r="D471" s="31"/>
     </row>
     <row r="472" ht="14.25" customHeight="1">
-      <c r="A472" s="30"/>
-      <c r="B472" s="31"/>
-      <c r="C472" s="30"/>
-      <c r="D472" s="30"/>
+      <c r="A472" s="31"/>
+      <c r="B472" s="32"/>
+      <c r="C472" s="31"/>
+      <c r="D472" s="31"/>
     </row>
     <row r="473" ht="14.25" customHeight="1">
-      <c r="A473" s="30"/>
-      <c r="B473" s="31"/>
-      <c r="C473" s="30"/>
-      <c r="D473" s="30"/>
+      <c r="A473" s="31"/>
+      <c r="B473" s="32"/>
+      <c r="C473" s="31"/>
+      <c r="D473" s="31"/>
     </row>
     <row r="474" ht="14.25" customHeight="1">
-      <c r="A474" s="30"/>
-      <c r="B474" s="31"/>
-      <c r="C474" s="30"/>
-      <c r="D474" s="30"/>
+      <c r="A474" s="31"/>
+      <c r="B474" s="32"/>
+      <c r="C474" s="31"/>
+      <c r="D474" s="31"/>
     </row>
     <row r="475" ht="14.25" customHeight="1">
-      <c r="A475" s="30"/>
-      <c r="B475" s="31"/>
-      <c r="C475" s="30"/>
-      <c r="D475" s="30"/>
+      <c r="A475" s="31"/>
+      <c r="B475" s="32"/>
+      <c r="C475" s="31"/>
+      <c r="D475" s="31"/>
     </row>
     <row r="476" ht="14.25" customHeight="1">
-      <c r="A476" s="30"/>
-      <c r="B476" s="31"/>
-      <c r="C476" s="30"/>
-      <c r="D476" s="30"/>
+      <c r="A476" s="31"/>
+      <c r="B476" s="32"/>
+      <c r="C476" s="31"/>
+      <c r="D476" s="31"/>
     </row>
     <row r="477" ht="14.25" customHeight="1">
-      <c r="A477" s="30"/>
-      <c r="B477" s="31"/>
-      <c r="C477" s="30"/>
-      <c r="D477" s="30"/>
+      <c r="A477" s="31"/>
+      <c r="B477" s="32"/>
+      <c r="C477" s="31"/>
+      <c r="D477" s="31"/>
     </row>
     <row r="478" ht="14.25" customHeight="1">
-      <c r="A478" s="30"/>
-      <c r="B478" s="31"/>
-      <c r="C478" s="30"/>
-      <c r="D478" s="30"/>
+      <c r="A478" s="31"/>
+      <c r="B478" s="32"/>
+      <c r="C478" s="31"/>
+      <c r="D478" s="31"/>
     </row>
     <row r="479" ht="14.25" customHeight="1">
-      <c r="A479" s="30"/>
-      <c r="B479" s="31"/>
-      <c r="C479" s="30"/>
-      <c r="D479" s="30"/>
+      <c r="A479" s="31"/>
+      <c r="B479" s="32"/>
+      <c r="C479" s="31"/>
+      <c r="D479" s="31"/>
     </row>
     <row r="480" ht="14.25" customHeight="1">
-      <c r="A480" s="30"/>
-      <c r="B480" s="31"/>
-      <c r="C480" s="30"/>
-      <c r="D480" s="30"/>
+      <c r="A480" s="31"/>
+      <c r="B480" s="32"/>
+      <c r="C480" s="31"/>
+      <c r="D480" s="31"/>
     </row>
     <row r="481" ht="14.25" customHeight="1">
-      <c r="A481" s="30"/>
-      <c r="B481" s="31"/>
-      <c r="C481" s="30"/>
-      <c r="D481" s="30"/>
+      <c r="A481" s="31"/>
+      <c r="B481" s="32"/>
+      <c r="C481" s="31"/>
+      <c r="D481" s="31"/>
     </row>
     <row r="482" ht="14.25" customHeight="1">
-      <c r="A482" s="30"/>
-      <c r="B482" s="31"/>
-      <c r="C482" s="30"/>
-      <c r="D482" s="30"/>
+      <c r="A482" s="31"/>
+      <c r="B482" s="32"/>
+      <c r="C482" s="31"/>
+      <c r="D482" s="31"/>
     </row>
     <row r="483" ht="14.25" customHeight="1">
-      <c r="A483" s="30"/>
-      <c r="B483" s="31"/>
-      <c r="C483" s="30"/>
-      <c r="D483" s="30"/>
+      <c r="A483" s="31"/>
+      <c r="B483" s="32"/>
+      <c r="C483" s="31"/>
+      <c r="D483" s="31"/>
     </row>
     <row r="484" ht="14.25" customHeight="1">
-      <c r="A484" s="30"/>
-      <c r="B484" s="31"/>
-      <c r="C484" s="30"/>
-      <c r="D484" s="30"/>
+      <c r="A484" s="31"/>
+      <c r="B484" s="32"/>
+      <c r="C484" s="31"/>
+      <c r="D484" s="31"/>
     </row>
     <row r="485" ht="14.25" customHeight="1">
-      <c r="A485" s="30"/>
-      <c r="B485" s="31"/>
-      <c r="C485" s="30"/>
-      <c r="D485" s="30"/>
+      <c r="A485" s="31"/>
+      <c r="B485" s="32"/>
+      <c r="C485" s="31"/>
+      <c r="D485" s="31"/>
     </row>
     <row r="486" ht="14.25" customHeight="1">
-      <c r="A486" s="30"/>
-      <c r="B486" s="31"/>
-      <c r="C486" s="30"/>
-      <c r="D486" s="30"/>
+      <c r="A486" s="31"/>
+      <c r="B486" s="32"/>
+      <c r="C486" s="31"/>
+      <c r="D486" s="31"/>
     </row>
     <row r="487" ht="14.25" customHeight="1">
-      <c r="A487" s="30"/>
-      <c r="B487" s="31"/>
-      <c r="C487" s="30"/>
-      <c r="D487" s="30"/>
+      <c r="A487" s="31"/>
+      <c r="B487" s="32"/>
+      <c r="C487" s="31"/>
+      <c r="D487" s="31"/>
     </row>
     <row r="488" ht="14.25" customHeight="1">
-      <c r="A488" s="30"/>
-      <c r="B488" s="31"/>
-      <c r="C488" s="30"/>
-      <c r="D488" s="30"/>
+      <c r="A488" s="31"/>
+      <c r="B488" s="32"/>
+      <c r="C488" s="31"/>
+      <c r="D488" s="31"/>
     </row>
     <row r="489" ht="14.25" customHeight="1">
-      <c r="A489" s="30"/>
-      <c r="B489" s="31"/>
-      <c r="C489" s="30"/>
-      <c r="D489" s="30"/>
+      <c r="A489" s="31"/>
+      <c r="B489" s="32"/>
+      <c r="C489" s="31"/>
+      <c r="D489" s="31"/>
     </row>
     <row r="490" ht="14.25" customHeight="1">
-      <c r="A490" s="30"/>
-      <c r="B490" s="31"/>
-      <c r="C490" s="30"/>
-      <c r="D490" s="30"/>
+      <c r="A490" s="31"/>
+      <c r="B490" s="32"/>
+      <c r="C490" s="31"/>
+      <c r="D490" s="31"/>
     </row>
     <row r="491" ht="14.25" customHeight="1">
-      <c r="A491" s="30"/>
-      <c r="B491" s="31"/>
-      <c r="C491" s="30"/>
-      <c r="D491" s="30"/>
+      <c r="A491" s="31"/>
+      <c r="B491" s="32"/>
+      <c r="C491" s="31"/>
+      <c r="D491" s="31"/>
     </row>
     <row r="492" ht="14.25" customHeight="1">
-      <c r="A492" s="30"/>
-      <c r="B492" s="31"/>
-      <c r="C492" s="30"/>
-      <c r="D492" s="30"/>
+      <c r="A492" s="31"/>
+      <c r="B492" s="32"/>
+      <c r="C492" s="31"/>
+      <c r="D492" s="31"/>
     </row>
     <row r="493" ht="14.25" customHeight="1">
-      <c r="A493" s="30"/>
-      <c r="B493" s="31"/>
-      <c r="C493" s="30"/>
-      <c r="D493" s="30"/>
+      <c r="A493" s="31"/>
+      <c r="B493" s="32"/>
+      <c r="C493" s="31"/>
+      <c r="D493" s="31"/>
     </row>
     <row r="494" ht="14.25" customHeight="1">
-      <c r="A494" s="30"/>
-      <c r="B494" s="31"/>
-      <c r="C494" s="30"/>
-      <c r="D494" s="30"/>
+      <c r="A494" s="31"/>
+      <c r="B494" s="32"/>
+      <c r="C494" s="31"/>
+      <c r="D494" s="31"/>
     </row>
     <row r="495" ht="14.25" customHeight="1">
-      <c r="A495" s="30"/>
-      <c r="B495" s="31"/>
-      <c r="C495" s="30"/>
-      <c r="D495" s="30"/>
+      <c r="A495" s="31"/>
+      <c r="B495" s="32"/>
+      <c r="C495" s="31"/>
+      <c r="D495" s="31"/>
     </row>
     <row r="496" ht="14.25" customHeight="1">
-      <c r="A496" s="30"/>
-      <c r="B496" s="31"/>
-      <c r="C496" s="30"/>
-      <c r="D496" s="30"/>
+      <c r="A496" s="31"/>
+      <c r="B496" s="32"/>
+      <c r="C496" s="31"/>
+      <c r="D496" s="31"/>
     </row>
     <row r="497" ht="14.25" customHeight="1">
-      <c r="A497" s="30"/>
-      <c r="B497" s="31"/>
-      <c r="C497" s="30"/>
-      <c r="D497" s="30"/>
+      <c r="A497" s="31"/>
+      <c r="B497" s="32"/>
+      <c r="C497" s="31"/>
+      <c r="D497" s="31"/>
     </row>
     <row r="498" ht="14.25" customHeight="1">
-      <c r="A498" s="30"/>
-      <c r="B498" s="31"/>
-      <c r="C498" s="30"/>
-      <c r="D498" s="30"/>
+      <c r="A498" s="31"/>
+      <c r="B498" s="32"/>
+      <c r="C498" s="31"/>
+      <c r="D498" s="31"/>
     </row>
     <row r="499" ht="14.25" customHeight="1">
-      <c r="A499" s="30"/>
-      <c r="B499" s="31"/>
-      <c r="C499" s="30"/>
-      <c r="D499" s="30"/>
+      <c r="A499" s="31"/>
+      <c r="B499" s="32"/>
+      <c r="C499" s="31"/>
+      <c r="D499" s="31"/>
     </row>
     <row r="500" ht="14.25" customHeight="1">
-      <c r="A500" s="30"/>
-      <c r="B500" s="31"/>
-      <c r="C500" s="30"/>
-      <c r="D500" s="30"/>
+      <c r="A500" s="31"/>
+      <c r="B500" s="32"/>
+      <c r="C500" s="31"/>
+      <c r="D500" s="31"/>
     </row>
     <row r="501" ht="14.25" customHeight="1">
-      <c r="A501" s="30"/>
-      <c r="B501" s="31"/>
-      <c r="C501" s="30"/>
-      <c r="D501" s="30"/>
+      <c r="A501" s="31"/>
+      <c r="B501" s="32"/>
+      <c r="C501" s="31"/>
+      <c r="D501" s="31"/>
     </row>
     <row r="502" ht="14.25" customHeight="1">
-      <c r="A502" s="30"/>
-      <c r="B502" s="31"/>
-      <c r="C502" s="30"/>
-      <c r="D502" s="30"/>
+      <c r="A502" s="31"/>
+      <c r="B502" s="32"/>
+      <c r="C502" s="31"/>
+      <c r="D502" s="31"/>
     </row>
     <row r="503" ht="14.25" customHeight="1">
-      <c r="A503" s="30"/>
-      <c r="B503" s="31"/>
-      <c r="C503" s="30"/>
-      <c r="D503" s="30"/>
+      <c r="A503" s="31"/>
+      <c r="B503" s="32"/>
+      <c r="C503" s="31"/>
+      <c r="D503" s="31"/>
     </row>
     <row r="504" ht="14.25" customHeight="1">
-      <c r="A504" s="30"/>
-      <c r="B504" s="31"/>
-      <c r="C504" s="30"/>
-      <c r="D504" s="30"/>
+      <c r="A504" s="31"/>
+      <c r="B504" s="32"/>
+      <c r="C504" s="31"/>
+      <c r="D504" s="31"/>
     </row>
     <row r="505" ht="14.25" customHeight="1">
-      <c r="A505" s="30"/>
-      <c r="B505" s="31"/>
-      <c r="C505" s="30"/>
-      <c r="D505" s="30"/>
+      <c r="A505" s="31"/>
+      <c r="B505" s="32"/>
+      <c r="C505" s="31"/>
+      <c r="D505" s="31"/>
     </row>
     <row r="506" ht="14.25" customHeight="1">
-      <c r="A506" s="30"/>
-      <c r="B506" s="31"/>
-      <c r="C506" s="30"/>
-      <c r="D506" s="30"/>
+      <c r="A506" s="31"/>
+      <c r="B506" s="32"/>
+      <c r="C506" s="31"/>
+      <c r="D506" s="31"/>
     </row>
     <row r="507" ht="14.25" customHeight="1">
-      <c r="A507" s="30"/>
-      <c r="B507" s="31"/>
-      <c r="C507" s="30"/>
-      <c r="D507" s="30"/>
+      <c r="A507" s="31"/>
+      <c r="B507" s="32"/>
+      <c r="C507" s="31"/>
+      <c r="D507" s="31"/>
     </row>
     <row r="508" ht="14.25" customHeight="1">
-      <c r="A508" s="30"/>
-      <c r="B508" s="31"/>
-      <c r="C508" s="30"/>
-      <c r="D508" s="30"/>
+      <c r="A508" s="31"/>
+      <c r="B508" s="32"/>
+      <c r="C508" s="31"/>
+      <c r="D508" s="31"/>
     </row>
     <row r="509" ht="14.25" customHeight="1">
-      <c r="A509" s="30"/>
-      <c r="B509" s="31"/>
-      <c r="C509" s="30"/>
-      <c r="D509" s="30"/>
+      <c r="A509" s="31"/>
+      <c r="B509" s="32"/>
+      <c r="C509" s="31"/>
+      <c r="D509" s="31"/>
     </row>
     <row r="510" ht="14.25" customHeight="1">
-      <c r="A510" s="30"/>
-      <c r="B510" s="31"/>
-      <c r="C510" s="30"/>
-      <c r="D510" s="30"/>
+      <c r="A510" s="31"/>
+      <c r="B510" s="32"/>
+      <c r="C510" s="31"/>
+      <c r="D510" s="31"/>
     </row>
     <row r="511" ht="14.25" customHeight="1">
-      <c r="A511" s="30"/>
-      <c r="B511" s="31"/>
-      <c r="C511" s="30"/>
-      <c r="D511" s="30"/>
+      <c r="A511" s="31"/>
+      <c r="B511" s="32"/>
+      <c r="C511" s="31"/>
+      <c r="D511" s="31"/>
     </row>
     <row r="512" ht="14.25" customHeight="1">
-      <c r="A512" s="30"/>
-      <c r="B512" s="31"/>
-      <c r="C512" s="30"/>
-      <c r="D512" s="30"/>
+      <c r="A512" s="31"/>
+      <c r="B512" s="32"/>
+      <c r="C512" s="31"/>
+      <c r="D512" s="31"/>
     </row>
     <row r="513" ht="14.25" customHeight="1">
-      <c r="A513" s="30"/>
-      <c r="B513" s="31"/>
-      <c r="C513" s="30"/>
-      <c r="D513" s="30"/>
+      <c r="A513" s="31"/>
+      <c r="B513" s="32"/>
+      <c r="C513" s="31"/>
+      <c r="D513" s="31"/>
     </row>
     <row r="514" ht="14.25" customHeight="1">
-      <c r="A514" s="30"/>
-      <c r="B514" s="31"/>
-      <c r="C514" s="30"/>
-      <c r="D514" s="30"/>
+      <c r="A514" s="31"/>
+      <c r="B514" s="32"/>
+      <c r="C514" s="31"/>
+      <c r="D514" s="31"/>
     </row>
     <row r="515" ht="14.25" customHeight="1">
-      <c r="A515" s="30"/>
-      <c r="B515" s="31"/>
-      <c r="C515" s="30"/>
-      <c r="D515" s="30"/>
+      <c r="A515" s="31"/>
+      <c r="B515" s="32"/>
+      <c r="C515" s="31"/>
+      <c r="D515" s="31"/>
     </row>
     <row r="516" ht="14.25" customHeight="1">
-      <c r="A516" s="30"/>
-      <c r="B516" s="31"/>
-      <c r="C516" s="30"/>
-      <c r="D516" s="30"/>
+      <c r="A516" s="31"/>
+      <c r="B516" s="32"/>
+      <c r="C516" s="31"/>
+      <c r="D516" s="31"/>
     </row>
     <row r="517" ht="14.25" customHeight="1">
-      <c r="A517" s="30"/>
-      <c r="B517" s="31"/>
-      <c r="C517" s="30"/>
-      <c r="D517" s="30"/>
+      <c r="A517" s="31"/>
+      <c r="B517" s="32"/>
+      <c r="C517" s="31"/>
+      <c r="D517" s="31"/>
     </row>
     <row r="518" ht="14.25" customHeight="1">
-      <c r="A518" s="30"/>
-      <c r="B518" s="31"/>
-      <c r="C518" s="30"/>
-      <c r="D518" s="30"/>
+      <c r="A518" s="31"/>
+      <c r="B518" s="32"/>
+      <c r="C518" s="31"/>
+      <c r="D518" s="31"/>
     </row>
     <row r="519" ht="14.25" customHeight="1">
-      <c r="A519" s="30"/>
-      <c r="B519" s="31"/>
-      <c r="C519" s="30"/>
-      <c r="D519" s="30"/>
+      <c r="A519" s="31"/>
+      <c r="B519" s="32"/>
+      <c r="C519" s="31"/>
+      <c r="D519" s="31"/>
     </row>
     <row r="520" ht="14.25" customHeight="1">
-      <c r="A520" s="30"/>
-      <c r="B520" s="31"/>
-      <c r="C520" s="30"/>
-      <c r="D520" s="30"/>
+      <c r="A520" s="31"/>
+      <c r="B520" s="32"/>
+      <c r="C520" s="31"/>
+      <c r="D520" s="31"/>
     </row>
     <row r="521" ht="14.25" customHeight="1">
-      <c r="A521" s="30"/>
-      <c r="B521" s="31"/>
-      <c r="C521" s="30"/>
-      <c r="D521" s="30"/>
+      <c r="A521" s="31"/>
+      <c r="B521" s="32"/>
+      <c r="C521" s="31"/>
+      <c r="D521" s="31"/>
     </row>
     <row r="522" ht="14.25" customHeight="1">
-      <c r="A522" s="30"/>
-      <c r="B522" s="31"/>
-      <c r="C522" s="30"/>
-      <c r="D522" s="30"/>
+      <c r="A522" s="31"/>
+      <c r="B522" s="32"/>
+      <c r="C522" s="31"/>
+      <c r="D522" s="31"/>
     </row>
     <row r="523" ht="14.25" customHeight="1">
-      <c r="A523" s="30"/>
-      <c r="B523" s="31"/>
-      <c r="C523" s="30"/>
-      <c r="D523" s="30"/>
+      <c r="A523" s="31"/>
+      <c r="B523" s="32"/>
+      <c r="C523" s="31"/>
+      <c r="D523" s="31"/>
     </row>
     <row r="524" ht="14.25" customHeight="1">
-      <c r="A524" s="30"/>
-      <c r="B524" s="31"/>
-      <c r="C524" s="30"/>
-      <c r="D524" s="30"/>
+      <c r="A524" s="31"/>
+      <c r="B524" s="32"/>
+      <c r="C524" s="31"/>
+      <c r="D524" s="31"/>
     </row>
     <row r="525" ht="14.25" customHeight="1">
-      <c r="A525" s="30"/>
-      <c r="B525" s="31"/>
-      <c r="C525" s="30"/>
-      <c r="D525" s="30"/>
+      <c r="A525" s="31"/>
+      <c r="B525" s="32"/>
+      <c r="C525" s="31"/>
+      <c r="D525" s="31"/>
     </row>
     <row r="526" ht="14.25" customHeight="1">
-      <c r="A526" s="30"/>
-      <c r="B526" s="31"/>
-      <c r="C526" s="30"/>
-      <c r="D526" s="30"/>
+      <c r="A526" s="31"/>
+      <c r="B526" s="32"/>
+      <c r="C526" s="31"/>
+      <c r="D526" s="31"/>
     </row>
     <row r="527" ht="14.25" customHeight="1">
-      <c r="A527" s="30"/>
-      <c r="B527" s="31"/>
-      <c r="C527" s="30"/>
-      <c r="D527" s="30"/>
+      <c r="A527" s="31"/>
+      <c r="B527" s="32"/>
+      <c r="C527" s="31"/>
+      <c r="D527" s="31"/>
     </row>
     <row r="528" ht="14.25" customHeight="1">
-      <c r="A528" s="30"/>
-      <c r="B528" s="31"/>
-      <c r="C528" s="30"/>
-      <c r="D528" s="30"/>
+      <c r="A528" s="31"/>
+      <c r="B528" s="32"/>
+      <c r="C528" s="31"/>
+      <c r="D528" s="31"/>
     </row>
     <row r="529" ht="14.25" customHeight="1">
-      <c r="A529" s="30"/>
-      <c r="B529" s="31"/>
-      <c r="C529" s="30"/>
-      <c r="D529" s="30"/>
+      <c r="A529" s="31"/>
+      <c r="B529" s="32"/>
+      <c r="C529" s="31"/>
+      <c r="D529" s="31"/>
     </row>
     <row r="530" ht="14.25" customHeight="1">
-      <c r="A530" s="30"/>
-      <c r="B530" s="31"/>
-      <c r="C530" s="30"/>
-      <c r="D530" s="30"/>
+      <c r="A530" s="31"/>
+      <c r="B530" s="32"/>
+      <c r="C530" s="31"/>
+      <c r="D530" s="31"/>
     </row>
     <row r="531" ht="14.25" customHeight="1">
-      <c r="A531" s="30"/>
-      <c r="B531" s="31"/>
-      <c r="C531" s="30"/>
-      <c r="D531" s="30"/>
+      <c r="A531" s="31"/>
+      <c r="B531" s="32"/>
+      <c r="C531" s="31"/>
+      <c r="D531" s="31"/>
     </row>
     <row r="532" ht="14.25" customHeight="1">
-      <c r="A532" s="30"/>
-      <c r="B532" s="31"/>
-      <c r="C532" s="30"/>
-      <c r="D532" s="30"/>
+      <c r="A532" s="31"/>
+      <c r="B532" s="32"/>
+      <c r="C532" s="31"/>
+      <c r="D532" s="31"/>
     </row>
     <row r="533" ht="14.25" customHeight="1">
-      <c r="A533" s="30"/>
-      <c r="B533" s="31"/>
-      <c r="C533" s="30"/>
-      <c r="D533" s="30"/>
+      <c r="A533" s="31"/>
+      <c r="B533" s="32"/>
+      <c r="C533" s="31"/>
+      <c r="D533" s="31"/>
     </row>
     <row r="534" ht="14.25" customHeight="1">
-      <c r="A534" s="30"/>
-      <c r="B534" s="31"/>
-      <c r="C534" s="30"/>
-      <c r="D534" s="30"/>
+      <c r="A534" s="31"/>
+      <c r="B534" s="32"/>
+      <c r="C534" s="31"/>
+      <c r="D534" s="31"/>
     </row>
     <row r="535" ht="14.25" customHeight="1">
-      <c r="A535" s="30"/>
-      <c r="B535" s="31"/>
-      <c r="C535" s="30"/>
-      <c r="D535" s="30"/>
+      <c r="A535" s="31"/>
+      <c r="B535" s="32"/>
+      <c r="C535" s="31"/>
+      <c r="D535" s="31"/>
     </row>
     <row r="536" ht="14.25" customHeight="1">
-      <c r="A536" s="30"/>
-      <c r="B536" s="31"/>
-      <c r="C536" s="30"/>
-      <c r="D536" s="30"/>
+      <c r="A536" s="31"/>
+      <c r="B536" s="32"/>
+      <c r="C536" s="31"/>
+      <c r="D536" s="31"/>
     </row>
     <row r="537" ht="14.25" customHeight="1">
-      <c r="A537" s="30"/>
-      <c r="B537" s="31"/>
-      <c r="C537" s="30"/>
-      <c r="D537" s="30"/>
+      <c r="A537" s="31"/>
+      <c r="B537" s="32"/>
+      <c r="C537" s="31"/>
+      <c r="D537" s="31"/>
     </row>
     <row r="538" ht="14.25" customHeight="1">
-      <c r="A538" s="30"/>
-      <c r="B538" s="31"/>
-      <c r="C538" s="30"/>
-      <c r="D538" s="30"/>
+      <c r="A538" s="31"/>
+      <c r="B538" s="32"/>
+      <c r="C538" s="31"/>
+      <c r="D538" s="31"/>
     </row>
     <row r="539" ht="14.25" customHeight="1">
-      <c r="A539" s="30"/>
-      <c r="B539" s="31"/>
-      <c r="C539" s="30"/>
-      <c r="D539" s="30"/>
+      <c r="A539" s="31"/>
+      <c r="B539" s="32"/>
+      <c r="C539" s="31"/>
+      <c r="D539" s="31"/>
     </row>
     <row r="540" ht="14.25" customHeight="1">
-      <c r="A540" s="30"/>
-      <c r="B540" s="31"/>
-      <c r="C540" s="30"/>
-      <c r="D540" s="30"/>
+      <c r="A540" s="31"/>
+      <c r="B540" s="32"/>
+      <c r="C540" s="31"/>
+      <c r="D540" s="31"/>
     </row>
     <row r="541" ht="14.25" customHeight="1">
-      <c r="A541" s="30"/>
-      <c r="B541" s="31"/>
-      <c r="C541" s="30"/>
-      <c r="D541" s="30"/>
+      <c r="A541" s="31"/>
+      <c r="B541" s="32"/>
+      <c r="C541" s="31"/>
+      <c r="D541" s="31"/>
     </row>
     <row r="542" ht="14.25" customHeight="1">
-      <c r="A542" s="30"/>
-      <c r="B542" s="31"/>
-      <c r="C542" s="30"/>
-      <c r="D542" s="30"/>
+      <c r="A542" s="31"/>
+      <c r="B542" s="32"/>
+      <c r="C542" s="31"/>
+      <c r="D542" s="31"/>
     </row>
     <row r="543" ht="14.25" customHeight="1">
-      <c r="A543" s="30"/>
-      <c r="B543" s="31"/>
-      <c r="C543" s="30"/>
-      <c r="D543" s="30"/>
+      <c r="A543" s="31"/>
+      <c r="B543" s="32"/>
+      <c r="C543" s="31"/>
+      <c r="D543" s="31"/>
     </row>
     <row r="544" ht="14.25" customHeight="1">
-      <c r="A544" s="30"/>
-      <c r="B544" s="31"/>
-      <c r="C544" s="30"/>
-      <c r="D544" s="30"/>
+      <c r="A544" s="31"/>
+      <c r="B544" s="32"/>
+      <c r="C544" s="31"/>
+      <c r="D544" s="31"/>
     </row>
     <row r="545" ht="14.25" customHeight="1">
-      <c r="A545" s="30"/>
-      <c r="B545" s="31"/>
-      <c r="C545" s="30"/>
-      <c r="D545" s="30"/>
+      <c r="A545" s="31"/>
+      <c r="B545" s="32"/>
+      <c r="C545" s="31"/>
+      <c r="D545" s="31"/>
     </row>
     <row r="546" ht="14.25" customHeight="1">
-      <c r="A546" s="30"/>
-      <c r="B546" s="31"/>
-      <c r="C546" s="30"/>
-      <c r="D546" s="30"/>
+      <c r="A546" s="31"/>
+      <c r="B546" s="32"/>
+      <c r="C546" s="31"/>
+      <c r="D546" s="31"/>
     </row>
     <row r="547" ht="14.25" customHeight="1">
-      <c r="A547" s="30"/>
-      <c r="B547" s="31"/>
-      <c r="C547" s="30"/>
-      <c r="D547" s="30"/>
+      <c r="A547" s="31"/>
+      <c r="B547" s="32"/>
+      <c r="C547" s="31"/>
+      <c r="D547" s="31"/>
     </row>
     <row r="548" ht="14.25" customHeight="1">
-      <c r="A548" s="30"/>
-      <c r="B548" s="31"/>
-      <c r="C548" s="30"/>
-      <c r="D548" s="30"/>
+      <c r="A548" s="31"/>
+      <c r="B548" s="32"/>
+      <c r="C548" s="31"/>
+      <c r="D548" s="31"/>
     </row>
     <row r="549" ht="14.25" customHeight="1">
-      <c r="A549" s="30"/>
-      <c r="B549" s="31"/>
-      <c r="C549" s="30"/>
-      <c r="D549" s="30"/>
+      <c r="A549" s="31"/>
+      <c r="B549" s="32"/>
+      <c r="C549" s="31"/>
+      <c r="D549" s="31"/>
     </row>
     <row r="550" ht="14.25" customHeight="1">
-      <c r="A550" s="30"/>
-      <c r="B550" s="31"/>
-      <c r="C550" s="30"/>
-      <c r="D550" s="30"/>
+      <c r="A550" s="31"/>
+      <c r="B550" s="32"/>
+      <c r="C550" s="31"/>
+      <c r="D550" s="31"/>
     </row>
     <row r="551" ht="14.25" customHeight="1">
-      <c r="A551" s="30"/>
-      <c r="B551" s="31"/>
-      <c r="C551" s="30"/>
-      <c r="D551" s="30"/>
+      <c r="A551" s="31"/>
+      <c r="B551" s="32"/>
+      <c r="C551" s="31"/>
+      <c r="D551" s="31"/>
     </row>
     <row r="552" ht="14.25" customHeight="1">
-      <c r="A552" s="30"/>
-      <c r="B552" s="31"/>
-      <c r="C552" s="30"/>
-      <c r="D552" s="30"/>
+      <c r="A552" s="31"/>
+      <c r="B552" s="32"/>
+      <c r="C552" s="31"/>
+      <c r="D552" s="31"/>
     </row>
     <row r="553" ht="14.25" customHeight="1">
-      <c r="A553" s="30"/>
-      <c r="B553" s="31"/>
-      <c r="C553" s="30"/>
-      <c r="D553" s="30"/>
+      <c r="A553" s="31"/>
+      <c r="B553" s="32"/>
+      <c r="C553" s="31"/>
+      <c r="D553" s="31"/>
     </row>
     <row r="554" ht="14.25" customHeight="1">
-      <c r="A554" s="30"/>
-      <c r="B554" s="31"/>
-      <c r="C554" s="30"/>
-      <c r="D554" s="30"/>
+      <c r="A554" s="31"/>
+      <c r="B554" s="32"/>
+      <c r="C554" s="31"/>
+      <c r="D554" s="31"/>
     </row>
     <row r="555" ht="14.25" customHeight="1">
-      <c r="A555" s="30"/>
-      <c r="B555" s="31"/>
-      <c r="C555" s="30"/>
-      <c r="D555" s="30"/>
+      <c r="A555" s="31"/>
+      <c r="B555" s="32"/>
+      <c r="C555" s="31"/>
+      <c r="D555" s="31"/>
     </row>
     <row r="556" ht="14.25" customHeight="1">
-      <c r="A556" s="30"/>
-      <c r="B556" s="31"/>
-      <c r="C556" s="30"/>
-      <c r="D556" s="30"/>
+      <c r="A556" s="31"/>
+      <c r="B556" s="32"/>
+      <c r="C556" s="31"/>
+      <c r="D556" s="31"/>
     </row>
     <row r="557" ht="14.25" customHeight="1">
-      <c r="A557" s="30"/>
-      <c r="B557" s="31"/>
-      <c r="C557" s="30"/>
-      <c r="D557" s="30"/>
+      <c r="A557" s="31"/>
+      <c r="B557" s="32"/>
+      <c r="C557" s="31"/>
+      <c r="D557" s="31"/>
     </row>
     <row r="558" ht="14.25" customHeight="1">
-      <c r="A558" s="30"/>
-      <c r="B558" s="31"/>
-      <c r="C558" s="30"/>
-      <c r="D558" s="30"/>
+      <c r="A558" s="31"/>
+      <c r="B558" s="32"/>
+      <c r="C558" s="31"/>
+      <c r="D558" s="31"/>
     </row>
     <row r="559" ht="14.25" customHeight="1">
-      <c r="A559" s="30"/>
-      <c r="B559" s="31"/>
-      <c r="C559" s="30"/>
-      <c r="D559" s="30"/>
+      <c r="A559" s="31"/>
+      <c r="B559" s="32"/>
+      <c r="C559" s="31"/>
+      <c r="D559" s="31"/>
     </row>
     <row r="560" ht="14.25" customHeight="1">
-      <c r="A560" s="30"/>
-      <c r="B560" s="31"/>
-      <c r="C560" s="30"/>
-      <c r="D560" s="30"/>
+      <c r="A560" s="31"/>
+      <c r="B560" s="32"/>
+      <c r="C560" s="31"/>
+      <c r="D560" s="31"/>
     </row>
     <row r="561" ht="14.25" customHeight="1">
-      <c r="A561" s="30"/>
-      <c r="B561" s="31"/>
-      <c r="C561" s="30"/>
-      <c r="D561" s="30"/>
+      <c r="A561" s="31"/>
+      <c r="B561" s="32"/>
+      <c r="C561" s="31"/>
+      <c r="D561" s="31"/>
     </row>
     <row r="562" ht="14.25" customHeight="1">
-      <c r="A562" s="30"/>
-      <c r="B562" s="31"/>
-      <c r="C562" s="30"/>
-      <c r="D562" s="30"/>
+      <c r="A562" s="31"/>
+      <c r="B562" s="32"/>
+      <c r="C562" s="31"/>
+      <c r="D562" s="31"/>
     </row>
     <row r="563" ht="14.25" customHeight="1">
-      <c r="A563" s="30"/>
-      <c r="B563" s="31"/>
-      <c r="C563" s="30"/>
-      <c r="D563" s="30"/>
+      <c r="A563" s="31"/>
+      <c r="B563" s="32"/>
+      <c r="C563" s="31"/>
+      <c r="D563" s="31"/>
     </row>
     <row r="564" ht="14.25" customHeight="1">
-      <c r="A564" s="30"/>
-      <c r="B564" s="31"/>
-      <c r="C564" s="30"/>
-      <c r="D564" s="30"/>
+      <c r="A564" s="31"/>
+      <c r="B564" s="32"/>
+      <c r="C564" s="31"/>
+      <c r="D564" s="31"/>
     </row>
     <row r="565" ht="14.25" customHeight="1">
-      <c r="A565" s="30"/>
-      <c r="B565" s="31"/>
-      <c r="C565" s="30"/>
-      <c r="D565" s="30"/>
+      <c r="A565" s="31"/>
+      <c r="B565" s="32"/>
+      <c r="C565" s="31"/>
+      <c r="D565" s="31"/>
     </row>
     <row r="566" ht="14.25" customHeight="1">
-      <c r="A566" s="30"/>
-      <c r="B566" s="31"/>
-      <c r="C566" s="30"/>
-      <c r="D566" s="30"/>
+      <c r="A566" s="31"/>
+      <c r="B566" s="32"/>
+      <c r="C566" s="31"/>
+      <c r="D566" s="31"/>
     </row>
     <row r="567" ht="14.25" customHeight="1">
-      <c r="A567" s="30"/>
-      <c r="B567" s="31"/>
-      <c r="C567" s="30"/>
-      <c r="D567" s="30"/>
+      <c r="A567" s="31"/>
+      <c r="B567" s="32"/>
+      <c r="C567" s="31"/>
+      <c r="D567" s="31"/>
     </row>
     <row r="568" ht="14.25" customHeight="1">
-      <c r="A568" s="30"/>
-      <c r="B568" s="31"/>
-      <c r="C568" s="30"/>
-      <c r="D568" s="30"/>
+      <c r="A568" s="31"/>
+      <c r="B568" s="32"/>
+      <c r="C568" s="31"/>
+      <c r="D568" s="31"/>
     </row>
     <row r="569" ht="14.25" customHeight="1">
-      <c r="A569" s="30"/>
-      <c r="B569" s="31"/>
-      <c r="C569" s="30"/>
-      <c r="D569" s="30"/>
+      <c r="A569" s="31"/>
+      <c r="B569" s="32"/>
+      <c r="C569" s="31"/>
+      <c r="D569" s="31"/>
     </row>
     <row r="570" ht="14.25" customHeight="1">
-      <c r="A570" s="30"/>
-      <c r="B570" s="31"/>
-      <c r="C570" s="30"/>
-      <c r="D570" s="30"/>
+      <c r="A570" s="31"/>
+      <c r="B570" s="32"/>
+      <c r="C570" s="31"/>
+      <c r="D570" s="31"/>
     </row>
     <row r="571" ht="14.25" customHeight="1">
-      <c r="A571" s="30"/>
-      <c r="B571" s="31"/>
-      <c r="C571" s="30"/>
-      <c r="D571" s="30"/>
+      <c r="A571" s="31"/>
+      <c r="B571" s="32"/>
+      <c r="C571" s="31"/>
+      <c r="D571" s="31"/>
     </row>
     <row r="572" ht="14.25" customHeight="1">
-      <c r="A572" s="30"/>
-      <c r="B572" s="31"/>
-      <c r="C572" s="30"/>
-      <c r="D572" s="30"/>
+      <c r="A572" s="31"/>
+      <c r="B572" s="32"/>
+      <c r="C572" s="31"/>
+      <c r="D572" s="31"/>
     </row>
     <row r="573" ht="14.25" customHeight="1">
-      <c r="A573" s="30"/>
-      <c r="B573" s="31"/>
-      <c r="C573" s="30"/>
-      <c r="D573" s="30"/>
+      <c r="A573" s="31"/>
+      <c r="B573" s="32"/>
+      <c r="C573" s="31"/>
+      <c r="D573" s="31"/>
     </row>
     <row r="574" ht="14.25" customHeight="1">
-      <c r="A574" s="30"/>
-      <c r="B574" s="31"/>
-      <c r="C574" s="30"/>
-      <c r="D574" s="30"/>
+      <c r="A574" s="31"/>
+      <c r="B574" s="32"/>
+      <c r="C574" s="31"/>
+      <c r="D574" s="31"/>
     </row>
     <row r="575" ht="14.25" customHeight="1">
-      <c r="A575" s="30"/>
-      <c r="B575" s="31"/>
-      <c r="C575" s="30"/>
-      <c r="D575" s="30"/>
+      <c r="A575" s="31"/>
+      <c r="B575" s="32"/>
+      <c r="C575" s="31"/>
+      <c r="D575" s="31"/>
     </row>
     <row r="576" ht="14.25" customHeight="1">
-      <c r="A576" s="30"/>
-      <c r="B576" s="31"/>
-      <c r="C576" s="30"/>
-      <c r="D576" s="30"/>
+      <c r="A576" s="31"/>
+      <c r="B576" s="32"/>
+      <c r="C576" s="31"/>
+      <c r="D576" s="31"/>
     </row>
     <row r="577" ht="14.25" customHeight="1">
-      <c r="A577" s="30"/>
-      <c r="B577" s="31"/>
-      <c r="C577" s="30"/>
-      <c r="D577" s="30"/>
+      <c r="A577" s="31"/>
+      <c r="B577" s="32"/>
+      <c r="C577" s="31"/>
+      <c r="D577" s="31"/>
     </row>
     <row r="578" ht="14.25" customHeight="1">
-      <c r="A578" s="30"/>
-      <c r="B578" s="31"/>
-      <c r="C578" s="30"/>
-      <c r="D578" s="30"/>
+      <c r="A578" s="31"/>
+      <c r="B578" s="32"/>
+      <c r="C578" s="31"/>
+      <c r="D578" s="31"/>
     </row>
     <row r="579" ht="14.25" customHeight="1">
-      <c r="A579" s="30"/>
-      <c r="B579" s="31"/>
-      <c r="C579" s="30"/>
-      <c r="D579" s="30"/>
+      <c r="A579" s="31"/>
+      <c r="B579" s="32"/>
+      <c r="C579" s="31"/>
+      <c r="D579" s="31"/>
     </row>
     <row r="580" ht="14.25" customHeight="1">
-      <c r="A580" s="30"/>
-      <c r="B580" s="31"/>
-      <c r="C580" s="30"/>
-      <c r="D580" s="30"/>
+      <c r="A580" s="31"/>
+      <c r="B580" s="32"/>
+      <c r="C580" s="31"/>
+      <c r="D580" s="31"/>
     </row>
     <row r="581" ht="14.25" customHeight="1">
-      <c r="A581" s="30"/>
-      <c r="B581" s="31"/>
-      <c r="C581" s="30"/>
-      <c r="D581" s="30"/>
+      <c r="A581" s="31"/>
+      <c r="B581" s="32"/>
+      <c r="C581" s="31"/>
+      <c r="D581" s="31"/>
     </row>
     <row r="582" ht="14.25" customHeight="1">
-      <c r="A582" s="30"/>
-      <c r="B582" s="31"/>
-      <c r="C582" s="30"/>
-      <c r="D582" s="30"/>
+      <c r="A582" s="31"/>
+      <c r="B582" s="32"/>
+      <c r="C582" s="31"/>
+      <c r="D582" s="31"/>
     </row>
     <row r="583" ht="14.25" customHeight="1">
-      <c r="A583" s="30"/>
-      <c r="B583" s="31"/>
-      <c r="C583" s="30"/>
-      <c r="D583" s="30"/>
+      <c r="A583" s="31"/>
+      <c r="B583" s="32"/>
+      <c r="C583" s="31"/>
+      <c r="D583" s="31"/>
     </row>
     <row r="584" ht="14.25" customHeight="1">
-      <c r="A584" s="30"/>
-      <c r="B584" s="31"/>
-      <c r="C584" s="30"/>
-      <c r="D584" s="30"/>
+      <c r="A584" s="31"/>
+      <c r="B584" s="32"/>
+      <c r="C584" s="31"/>
+      <c r="D584" s="31"/>
     </row>
     <row r="585" ht="14.25" customHeight="1">
-      <c r="A585" s="30"/>
-      <c r="B585" s="31"/>
-      <c r="C585" s="30"/>
-      <c r="D585" s="30"/>
+      <c r="A585" s="31"/>
+      <c r="B585" s="32"/>
+      <c r="C585" s="31"/>
+      <c r="D585" s="31"/>
     </row>
     <row r="586" ht="14.25" customHeight="1">
-      <c r="A586" s="30"/>
-      <c r="B586" s="31"/>
-      <c r="C586" s="30"/>
-      <c r="D586" s="30"/>
+      <c r="A586" s="31"/>
+      <c r="B586" s="32"/>
+      <c r="C586" s="31"/>
+      <c r="D586" s="31"/>
     </row>
     <row r="587" ht="14.25" customHeight="1">
-      <c r="A587" s="30"/>
-      <c r="B587" s="31"/>
-      <c r="C587" s="30"/>
-      <c r="D587" s="30"/>
+      <c r="A587" s="31"/>
+      <c r="B587" s="32"/>
+      <c r="C587" s="31"/>
+      <c r="D587" s="31"/>
     </row>
     <row r="588" ht="14.25" customHeight="1">
-      <c r="A588" s="30"/>
-      <c r="B588" s="31"/>
-      <c r="C588" s="30"/>
-      <c r="D588" s="30"/>
+      <c r="A588" s="31"/>
+      <c r="B588" s="32"/>
+      <c r="C588" s="31"/>
+      <c r="D588" s="31"/>
     </row>
     <row r="589" ht="14.25" customHeight="1">
-      <c r="A589" s="30"/>
-      <c r="B589" s="31"/>
-      <c r="C589" s="30"/>
-      <c r="D589" s="30"/>
+      <c r="A589" s="31"/>
+      <c r="B589" s="32"/>
+      <c r="C589" s="31"/>
+      <c r="D589" s="31"/>
     </row>
     <row r="590" ht="14.25" customHeight="1">
-      <c r="A590" s="30"/>
-      <c r="B590" s="31"/>
-      <c r="C590" s="30"/>
-      <c r="D590" s="30"/>
+      <c r="A590" s="31"/>
+      <c r="B590" s="32"/>
+      <c r="C590" s="31"/>
+      <c r="D590" s="31"/>
     </row>
     <row r="591" ht="14.25" customHeight="1">
-      <c r="A591" s="30"/>
-      <c r="B591" s="31"/>
-      <c r="C591" s="30"/>
-      <c r="D591" s="30"/>
+      <c r="A591" s="31"/>
+      <c r="B591" s="32"/>
+      <c r="C591" s="31"/>
+      <c r="D591" s="31"/>
     </row>
     <row r="592" ht="14.25" customHeight="1">
-      <c r="A592" s="30"/>
-      <c r="B592" s="31"/>
-      <c r="C592" s="30"/>
-      <c r="D592" s="30"/>
+      <c r="A592" s="31"/>
+      <c r="B592" s="32"/>
+      <c r="C592" s="31"/>
+      <c r="D592" s="31"/>
     </row>
     <row r="593" ht="14.25" customHeight="1">
-      <c r="A593" s="30"/>
-      <c r="B593" s="31"/>
-      <c r="C593" s="30"/>
-      <c r="D593" s="30"/>
+      <c r="A593" s="31"/>
+      <c r="B593" s="32"/>
+      <c r="C593" s="31"/>
+      <c r="D593" s="31"/>
     </row>
     <row r="594" ht="14.25" customHeight="1">
-      <c r="A594" s="30"/>
-      <c r="B594" s="31"/>
-      <c r="C594" s="30"/>
-      <c r="D594" s="30"/>
+      <c r="A594" s="31"/>
+      <c r="B594" s="32"/>
+      <c r="C594" s="31"/>
+      <c r="D594" s="31"/>
     </row>
     <row r="595" ht="14.25" customHeight="1">
-      <c r="A595" s="30"/>
-      <c r="B595" s="31"/>
-      <c r="C595" s="30"/>
-      <c r="D595" s="30"/>
+      <c r="A595" s="31"/>
+      <c r="B595" s="32"/>
+      <c r="C595" s="31"/>
+      <c r="D595" s="31"/>
     </row>
     <row r="596" ht="15.75" customHeight="1"/>
     <row r="597" ht="15.75" customHeight="1"/>
@@ -11011,10 +11014,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>1099</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11029,45 +11032,45 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="32" t="s">
         <v>472</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="32" t="s">
         <v>473</v>
       </c>
-      <c r="E2" s="33" t="str">
+      <c r="E2" s="34" t="str">
         <f t="array" ref="E2">CONCATENATE(XLOOKUP($A2,Lotes!$A:$A,Lotes!$C:$C),"/",XLOOKUP($B2,Lotes!$A:$A,Lotes!$C:$C))</f>
         <v>J2304/H2162</v>
       </c>
-      <c r="F2" s="34" t="str">
+      <c r="F2" s="35" t="str">
         <f t="array" ref="F2">XLOOKUP($A2,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>10/28</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>383</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="36" t="s">
         <v>475</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="32" t="s">
         <v>476</v>
       </c>
-      <c r="E3" s="33" t="str">
+      <c r="E3" s="34" t="str">
         <f t="array" ref="E3">CONCATENATE(XLOOKUP($A3,Lotes!$A:$A,Lotes!$C:$C),"/",XLOOKUP($B3,Lotes!$A:$A,Lotes!$C:$C))</f>
         <v>J2304/J2267</v>
       </c>
-      <c r="F3" s="34" t="str">
+      <c r="F3" s="35" t="str">
         <f t="array" ref="F3">XLOOKUP($A3,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>10/28</v>
       </c>
@@ -11076,518 +11079,518 @@
       <c r="A4" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32" t="s">
         <v>428</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>429</v>
       </c>
-      <c r="E4" s="34" t="str">
+      <c r="E4" s="35" t="str">
         <f t="array" ref="E4">XLOOKUP($A4,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>2025210BLEFA</v>
       </c>
-      <c r="F4" s="34" t="str">
+      <c r="F4" s="35" t="str">
         <f t="array" ref="F4">XLOOKUP($A4,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>02/27</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32" t="s">
         <v>430</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>431</v>
       </c>
-      <c r="E5" s="34" t="str">
+      <c r="E5" s="35" t="str">
         <f t="array" ref="E5">XLOOKUP($A5,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>20241609BLEFL</v>
       </c>
-      <c r="F5" s="34" t="str">
+      <c r="F5" s="35" t="str">
         <f t="array" ref="F5">XLOOKUP($A5,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>09/26</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="32" t="s">
         <v>433</v>
       </c>
-      <c r="E6" s="34" t="str">
+      <c r="E6" s="35" t="str">
         <f t="array" ref="E6">XLOOKUP($A6,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>20252207BLEMA</v>
       </c>
-      <c r="F6" s="34" t="str">
+      <c r="F6" s="35" t="str">
         <f t="array" ref="F6">XLOOKUP($A6,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>07/27</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32" t="s">
         <v>434</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="32" t="s">
         <v>435</v>
       </c>
-      <c r="E7" s="34" t="str">
+      <c r="E7" s="35" t="str">
         <f t="array" ref="E7">XLOOKUP($A7,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>20252602BLESR</v>
       </c>
-      <c r="F7" s="34" t="str">
+      <c r="F7" s="35" t="str">
         <f t="array" ref="F7">XLOOKUP($A7,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>02/27</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>508</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="32" t="s">
         <v>436</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="32" t="s">
         <v>437</v>
       </c>
-      <c r="E8" s="34" t="str">
+      <c r="E8" s="35" t="str">
         <f t="array" ref="E8">XLOOKUP($A8,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>OLFA2508</v>
       </c>
-      <c r="F8" s="34" t="str">
+      <c r="F8" s="35" t="str">
         <f t="array" ref="F8">XLOOKUP($A8,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>08/27</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>511</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32" t="s">
         <v>438</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="32" t="s">
         <v>439</v>
       </c>
-      <c r="E9" s="34" t="str">
+      <c r="E9" s="35" t="str">
         <f t="array" ref="E9">XLOOKUP($A9,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>OLFL2510</v>
       </c>
-      <c r="F9" s="34" t="str">
+      <c r="F9" s="35" t="str">
         <f t="array" ref="F9">XLOOKUP($A9,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>10/27</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="32" t="s">
         <v>514</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="32" t="s">
         <v>440</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="32" t="s">
         <v>441</v>
       </c>
-      <c r="E10" s="34" t="str">
+      <c r="E10" s="35" t="str">
         <f t="array" ref="E10">XLOOKUP($A10,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>OLIN2508</v>
       </c>
-      <c r="F10" s="34" t="str">
+      <c r="F10" s="35" t="str">
         <f t="array" ref="F10">XLOOKUP($A10,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>08/27</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="32" t="s">
         <v>517</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32" t="s">
         <v>442</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="32" t="s">
         <v>443</v>
       </c>
-      <c r="E11" s="34" t="str">
+      <c r="E11" s="35" t="str">
         <f t="array" ref="E11">XLOOKUP($A11,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>OLLA2507</v>
       </c>
-      <c r="F11" s="34" t="str">
+      <c r="F11" s="35" t="str">
         <f t="array" ref="F11">XLOOKUP($A11,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>07/27</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="32" t="s">
         <v>520</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="32" t="s">
         <v>444</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="32" t="s">
         <v>445</v>
       </c>
-      <c r="E12" s="34" t="str">
+      <c r="E12" s="35" t="str">
         <f t="array" ref="E12">XLOOKUP($A12,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>OLMP2509</v>
       </c>
-      <c r="F12" s="34" t="str">
+      <c r="F12" s="35" t="str">
         <f t="array" ref="F12">XLOOKUP($A12,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>09/27</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>524</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="32" t="s">
         <v>446</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="32" t="s">
         <v>447</v>
       </c>
-      <c r="E13" s="34" t="str">
+      <c r="E13" s="35" t="str">
         <f t="array" ref="E13">XLOOKUP($A13,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>OLMC2509</v>
       </c>
-      <c r="F13" s="34" t="str">
+      <c r="F13" s="35" t="str">
         <f t="array" ref="F13">XLOOKUP($A13,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>09/27</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="32" t="s">
         <v>531</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="32" t="s">
         <v>448</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="32" t="s">
         <v>449</v>
       </c>
-      <c r="E14" s="34" t="str">
+      <c r="E14" s="35" t="str">
         <f t="array" ref="E14">XLOOKUP($A14,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>OLPV2510</v>
       </c>
-      <c r="F14" s="34" t="str">
+      <c r="F14" s="35" t="str">
         <f t="array" ref="F14">XLOOKUP($A14,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>10/27</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="32" t="s">
         <v>537</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="32" t="s">
         <v>450</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="32" t="s">
         <v>451</v>
       </c>
-      <c r="E15" s="34" t="str">
+      <c r="E15" s="35" t="str">
         <f t="array" ref="E15">XLOOKUP($A15,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>OLSR2508</v>
       </c>
-      <c r="F15" s="34" t="str">
+      <c r="F15" s="35" t="str">
         <f t="array" ref="F15">XLOOKUP($A15,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>08/27</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="32" t="s">
         <v>900</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="32"/>
+      <c r="C16" s="32" t="s">
         <v>481</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="32" t="s">
         <v>482</v>
       </c>
-      <c r="E16" s="34" t="str">
+      <c r="E16" s="35" t="str">
         <f t="array" ref="E16">XLOOKUP($A16,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>240105</v>
       </c>
-      <c r="F16" s="34" t="str">
+      <c r="F16" s="35" t="str">
         <f t="array" ref="F16">XLOOKUP($A16,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>11/27</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="32" t="s">
         <v>902</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32" t="s">
         <v>483</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="32" t="s">
         <v>484</v>
       </c>
-      <c r="E17" s="34" t="str">
+      <c r="E17" s="35" t="str">
         <f t="array" ref="E17">XLOOKUP($A17,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>250105</v>
       </c>
-      <c r="F17" s="34" t="str">
+      <c r="F17" s="35" t="str">
         <f t="array" ref="F17">XLOOKUP($A17,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>11/27</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="32" t="s">
         <v>905</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="32" t="s">
         <v>486</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="32" t="s">
         <v>487</v>
       </c>
-      <c r="E18" s="34" t="str">
+      <c r="E18" s="35" t="str">
         <f t="array" ref="E18">XLOOKUP($A18,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>240205</v>
       </c>
-      <c r="F18" s="34" t="str">
+      <c r="F18" s="35" t="str">
         <f t="array" ref="F18">XLOOKUP($A18,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>10/27</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="32" t="s">
         <v>908</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="32" t="s">
         <v>488</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="32" t="s">
         <v>489</v>
       </c>
-      <c r="E19" s="34" t="str">
+      <c r="E19" s="35" t="str">
         <f t="array" ref="E19">XLOOKUP($A19,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>240204</v>
       </c>
-      <c r="F19" s="34" t="str">
+      <c r="F19" s="35" t="str">
         <f t="array" ref="F19">XLOOKUP($A19,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>09/27</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="32" t="s">
         <v>914</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32" t="s">
         <v>490</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="32" t="s">
         <v>491</v>
       </c>
-      <c r="E20" s="34" t="str">
+      <c r="E20" s="35" t="str">
         <f t="array" ref="E20">XLOOKUP($A20,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>240303</v>
       </c>
-      <c r="F20" s="34" t="str">
+      <c r="F20" s="35" t="str">
         <f t="array" ref="F20">XLOOKUP($A20,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>08/28</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="32" t="s">
         <v>917</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="32" t="s">
         <v>492</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="32" t="s">
         <v>493</v>
       </c>
-      <c r="E21" s="34" t="str">
+      <c r="E21" s="35" t="str">
         <f t="array" ref="E21">XLOOKUP($A21,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>250302</v>
       </c>
-      <c r="F21" s="34" t="str">
+      <c r="F21" s="35" t="str">
         <f t="array" ref="F21">XLOOKUP($A21,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>07/28</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="32" t="s">
         <v>923</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="32" t="s">
         <v>494</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="32" t="s">
         <v>495</v>
       </c>
-      <c r="E22" s="34" t="str">
+      <c r="E22" s="35" t="str">
         <f t="array" ref="E22">XLOOKUP($A22,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>LEN89.0005</v>
       </c>
-      <c r="F22" s="34" t="str">
+      <c r="F22" s="35" t="str">
         <f t="array" ref="F22">XLOOKUP($A22,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>10/28</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="32" t="s">
         <v>496</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31" t="s">
+      <c r="B23" s="32"/>
+      <c r="C23" s="32" t="s">
         <v>496</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="32" t="s">
         <v>1100</v>
       </c>
-      <c r="E23" s="34" t="str">
+      <c r="E23" s="35" t="str">
         <f t="array" ref="E23">XLOOKUP($A23,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>250703</v>
       </c>
-      <c r="F23" s="34" t="str">
+      <c r="F23" s="35" t="str">
         <f t="array" ref="F23">XLOOKUP($A23,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>06/28</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36" t="s">
+      <c r="B24" s="37"/>
+      <c r="C24" s="37" t="s">
         <v>499</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="37" t="s">
         <v>500</v>
       </c>
-      <c r="E24" s="34" t="str">
+      <c r="E24" s="35" t="str">
         <f t="array" ref="E24">XLOOKUP($A24,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>20252602BLESR</v>
       </c>
-      <c r="F24" s="34" t="str">
+      <c r="F24" s="35" t="str">
         <f t="array" ref="F24">XLOOKUP($A24,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>02/27</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31" t="s">
+      <c r="B25" s="32"/>
+      <c r="C25" s="32" t="s">
         <v>466</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="32" t="s">
         <v>467</v>
       </c>
-      <c r="E25" s="34" t="str">
+      <c r="E25" s="35" t="str">
         <f t="array" ref="E25">XLOOKUP($A25,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>20241609BLEFL</v>
       </c>
-      <c r="F25" s="34" t="str">
+      <c r="F25" s="35" t="str">
         <f t="array" ref="F25">XLOOKUP($A25,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>09/26</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="32" t="s">
         <v>464</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="32" t="s">
         <v>465</v>
       </c>
-      <c r="E26" s="34" t="str">
+      <c r="E26" s="35" t="str">
         <f t="array" ref="E26">XLOOKUP($A26,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>2025210BLEFA</v>
       </c>
-      <c r="F26" s="34" t="str">
+      <c r="F26" s="35" t="str">
         <f t="array" ref="F26">XLOOKUP($A26,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>02/27</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31" t="s">
+      <c r="B27" s="32"/>
+      <c r="C27" s="32" t="s">
         <v>470</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="32" t="s">
         <v>471</v>
       </c>
-      <c r="E27" s="34" t="str">
+      <c r="E27" s="35" t="str">
         <f t="array" ref="E27">XLOOKUP($A27,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>20252207BLEMA</v>
       </c>
-      <c r="F27" s="34" t="str">
+      <c r="F27" s="35" t="str">
         <f t="array" ref="F27">XLOOKUP($A27,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>07/27</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="32" t="s">
         <v>479</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="32" t="s">
         <v>480</v>
       </c>
-      <c r="E28" s="34" t="str">
+      <c r="E28" s="35" t="str">
         <f t="array" ref="E28">XLOOKUP($A28,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>20240601BLEPE</v>
       </c>
-      <c r="F28" s="34" t="str">
+      <c r="F28" s="35" t="str">
         <f t="array" ref="F28">XLOOKUP($A28,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>06/26</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36" t="s">
+      <c r="B29" s="37"/>
+      <c r="C29" s="37" t="s">
         <v>468</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="37" t="s">
         <v>1101</v>
       </c>
-      <c r="E29" s="34" t="str">
+      <c r="E29" s="35" t="str">
         <f t="array" ref="E29">XLOOKUP($A29,Lotes!$A:$A,Lotes!$C:$C)</f>
         <v>20252207BLEMA</v>
       </c>
-      <c r="F29" s="34" t="str">
+      <c r="F29" s="35" t="str">
         <f t="array" ref="F29">XLOOKUP($A29,Lotes!$A:$A,Lotes!$D:$D)</f>
         <v>07/27</v>
       </c>
@@ -11627,12 +11630,12 @@
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="37"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
+      <c r="A64" s="38"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
     </row>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
@@ -11661,12 +11664,12 @@
     <row r="89" ht="15.75" customHeight="1"/>
     <row r="90" ht="15.75" customHeight="1"/>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="37"/>
-      <c r="B91" s="37"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="37"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="37"/>
+      <c r="A91" s="38"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="38"/>
     </row>
     <row r="92" ht="15.75" customHeight="1"/>
     <row r="93" ht="15.75" customHeight="1"/>

</xml_diff>